<commit_message>
added largest MC screen from BB
</commit_message>
<xml_diff>
--- a/Software.xlsx
+++ b/Software.xlsx
@@ -8,21 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Martin\code\models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F49EB951-D67B-40C9-BCBF-3C76E3375BD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B708DA89-E1DF-480D-A496-7719BA094BC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9630" yWindow="435" windowWidth="19665" windowHeight="15210" xr2:uid="{BF8D921A-3A39-424B-AF48-6465810DF752}"/>
+    <workbookView xWindow="8160" yWindow="75" windowWidth="20745" windowHeight="15540" xr2:uid="{BF8D921A-3A39-424B-AF48-6465810DF752}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
-    <sheet name="Gaming" sheetId="4" r:id="rId2"/>
-    <sheet name="Ecommerce" sheetId="3" r:id="rId3"/>
-    <sheet name="Fintech" sheetId="5" r:id="rId4"/>
-    <sheet name="Gig" sheetId="7" r:id="rId5"/>
-    <sheet name="Private" sheetId="6" r:id="rId6"/>
-    <sheet name="FX" sheetId="2" r:id="rId7"/>
+    <sheet name="Security" sheetId="8" r:id="rId2"/>
+    <sheet name="Gaming" sheetId="4" r:id="rId3"/>
+    <sheet name="Ecommerce" sheetId="3" r:id="rId4"/>
+    <sheet name="Fintech" sheetId="5" r:id="rId5"/>
+    <sheet name="Gig" sheetId="7" r:id="rId6"/>
+    <sheet name="Private" sheetId="6" r:id="rId7"/>
+    <sheet name="FX" sheetId="2" r:id="rId8"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId8"/>
     <externalReference r:id="rId9"/>
     <externalReference r:id="rId10"/>
     <externalReference r:id="rId11"/>
@@ -33,6 +33,7 @@
     <externalReference r:id="rId16"/>
     <externalReference r:id="rId17"/>
     <externalReference r:id="rId18"/>
+    <externalReference r:id="rId19"/>
   </externalReferences>
   <definedNames>
     <definedName name="HKD">FX!$C$3</definedName>
@@ -79,7 +80,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="163">
   <si>
     <t>Name</t>
   </si>
@@ -541,6 +542,33 @@
   </si>
   <si>
     <t>Q222</t>
+  </si>
+  <si>
+    <t>Agora</t>
+  </si>
+  <si>
+    <t>API</t>
+  </si>
+  <si>
+    <t>Dassault</t>
+  </si>
+  <si>
+    <t>DSY FP</t>
+  </si>
+  <si>
+    <t>VMWare</t>
+  </si>
+  <si>
+    <t>VMW</t>
+  </si>
+  <si>
+    <t>Main</t>
+  </si>
+  <si>
+    <t>CRWD</t>
+  </si>
+  <si>
+    <t>Crowdstrike</t>
   </si>
 </sst>
 </file>
@@ -783,7 +811,7 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -871,7 +899,7 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1226,10 +1254,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD51BEF3-80A6-4EBC-80AF-AC127A740620}">
-  <dimension ref="A1:H66"/>
+  <dimension ref="A1:H69"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1550,17 +1581,13 @@
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="1"/>
       <c r="B14" s="1" t="s">
-        <v>37</v>
+        <v>156</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D14" s="2">
-        <v>391.47</v>
-      </c>
-      <c r="E14" s="3">
-        <v>55690</v>
-      </c>
+        <v>157</v>
+      </c>
+      <c r="D14" s="2"/>
+      <c r="E14" s="3"/>
       <c r="F14" s="4"/>
       <c r="G14" s="4"/>
       <c r="H14" s="4"/>
@@ -1568,16 +1595,16 @@
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="1"/>
       <c r="B15" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D15" s="2">
-        <v>152.88</v>
+        <v>391.47</v>
       </c>
       <c r="E15" s="3">
-        <v>52828</v>
+        <v>55690</v>
       </c>
       <c r="F15" s="4"/>
       <c r="G15" s="4"/>
@@ -1586,16 +1613,16 @@
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="1"/>
       <c r="B16" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D16" s="2">
-        <v>200.8</v>
+        <v>152.88</v>
       </c>
       <c r="E16" s="3">
-        <v>52670</v>
+        <v>52828</v>
       </c>
       <c r="F16" s="4"/>
       <c r="G16" s="4"/>
@@ -1604,16 +1631,16 @@
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="1"/>
       <c r="B17" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D17" s="2">
-        <v>135.57</v>
+        <v>200.8</v>
       </c>
       <c r="E17" s="3">
-        <v>45920</v>
+        <v>52670</v>
       </c>
       <c r="F17" s="4"/>
       <c r="G17" s="4"/>
@@ -1622,16 +1649,16 @@
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="1"/>
       <c r="B18" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D18" s="2">
-        <v>203.73</v>
+        <v>135.57</v>
       </c>
       <c r="E18" s="3">
-        <v>45530</v>
+        <v>45920</v>
       </c>
       <c r="F18" s="4"/>
       <c r="G18" s="4"/>
@@ -1640,16 +1667,16 @@
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="1"/>
       <c r="B19" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D19" s="2">
-        <v>159.93</v>
+        <v>203.73</v>
       </c>
       <c r="E19" s="3">
-        <v>44900</v>
+        <v>45530</v>
       </c>
       <c r="F19" s="4"/>
       <c r="G19" s="4"/>
@@ -1658,16 +1685,16 @@
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="1"/>
       <c r="B20" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D20" s="2">
-        <v>160.03</v>
+        <v>159.93</v>
       </c>
       <c r="E20" s="3">
-        <v>40648</v>
+        <v>44900</v>
       </c>
       <c r="F20" s="4"/>
       <c r="G20" s="4"/>
@@ -1676,16 +1703,16 @@
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="1"/>
       <c r="B21" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D21" s="2">
-        <v>107.93</v>
+        <v>160.03</v>
       </c>
       <c r="E21" s="3">
-        <v>34000</v>
+        <v>40648</v>
       </c>
       <c r="F21" s="4"/>
       <c r="G21" s="4"/>
@@ -1694,13 +1721,13 @@
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="1"/>
       <c r="B22" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C22" s="1"/>
+        <v>158</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>159</v>
+      </c>
       <c r="D22" s="2"/>
-      <c r="E22" s="3">
-        <v>30000</v>
-      </c>
+      <c r="E22" s="3"/>
       <c r="F22" s="4"/>
       <c r="G22" s="4"/>
       <c r="H22" s="4"/>
@@ -1708,16 +1735,16 @@
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="1"/>
       <c r="B23" s="1" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D23" s="2">
-        <v>54.71</v>
+        <v>107.93</v>
       </c>
       <c r="E23" s="3">
-        <v>28410</v>
+        <v>34000</v>
       </c>
       <c r="F23" s="4"/>
       <c r="G23" s="4"/>
@@ -1726,12 +1753,12 @@
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="1"/>
       <c r="B24" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C24" s="1"/>
       <c r="D24" s="2"/>
       <c r="E24" s="3">
-        <v>27000</v>
+        <v>30000</v>
       </c>
       <c r="F24" s="4"/>
       <c r="G24" s="4"/>
@@ -1740,12 +1767,16 @@
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="1"/>
       <c r="B25" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="C25" s="1"/>
-      <c r="D25" s="2"/>
+        <v>57</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D25" s="2">
+        <v>54.71</v>
+      </c>
       <c r="E25" s="3">
-        <v>26000</v>
+        <v>28410</v>
       </c>
       <c r="F25" s="4"/>
       <c r="G25" s="4"/>
@@ -1754,16 +1785,12 @@
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" s="1"/>
       <c r="B26" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D26" s="2">
-        <v>236.61</v>
-      </c>
+        <v>59</v>
+      </c>
+      <c r="C26" s="1"/>
+      <c r="D26" s="2"/>
       <c r="E26" s="3">
-        <v>23190</v>
+        <v>27000</v>
       </c>
       <c r="F26" s="4"/>
       <c r="G26" s="4"/>
@@ -1772,16 +1799,12 @@
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" s="1"/>
       <c r="B27" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="D27" s="2">
-        <v>90.1</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="C27" s="1"/>
+      <c r="D27" s="2"/>
       <c r="E27" s="3">
-        <v>18840</v>
+        <v>26000</v>
       </c>
       <c r="F27" s="4"/>
       <c r="G27" s="4"/>
@@ -1790,16 +1813,16 @@
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" s="1"/>
       <c r="B28" s="1" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="D28" s="2">
-        <v>360.34</v>
+        <v>236.61</v>
       </c>
       <c r="E28" s="3">
-        <v>18140</v>
+        <v>23190</v>
       </c>
       <c r="F28" s="4"/>
       <c r="G28" s="4"/>
@@ -1808,16 +1831,16 @@
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" s="1"/>
       <c r="B29" s="1" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="D29" s="2">
-        <v>68.930000000000007</v>
+        <v>90.1</v>
       </c>
       <c r="E29" s="3">
-        <v>18053</v>
+        <v>18840</v>
       </c>
       <c r="F29" s="4"/>
       <c r="G29" s="4"/>
@@ -1826,16 +1849,16 @@
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" s="1"/>
       <c r="B30" s="1" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="D30" s="2">
-        <v>43.75</v>
+        <v>360.34</v>
       </c>
       <c r="E30" s="3">
-        <v>17180</v>
+        <v>18140</v>
       </c>
       <c r="F30" s="4"/>
       <c r="G30" s="4"/>
@@ -1843,41 +1866,35 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" s="1"/>
-      <c r="B31" s="5" t="s">
-        <v>76</v>
+      <c r="B31" s="1" t="s">
+        <v>72</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="D31" s="2">
-        <v>102.23</v>
-      </c>
-      <c r="E31" s="3"/>
-      <c r="F31" s="3">
-        <f>+[10]Main!$K$5-[10]Main!$K$6</f>
-        <v>3155</v>
-      </c>
-      <c r="G31" s="3">
-        <f>E31-F31</f>
-        <v>-3155</v>
-      </c>
-      <c r="H31" s="4" t="s">
-        <v>9</v>
-      </c>
+        <v>68.930000000000007</v>
+      </c>
+      <c r="E31" s="3">
+        <v>18053</v>
+      </c>
+      <c r="F31" s="4"/>
+      <c r="G31" s="4"/>
+      <c r="H31" s="4"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" s="1"/>
       <c r="B32" s="1" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="D32" s="2">
-        <v>40.44</v>
+        <v>43.75</v>
       </c>
       <c r="E32" s="3">
-        <v>16810</v>
+        <v>17180</v>
       </c>
       <c r="F32" s="4"/>
       <c r="G32" s="4"/>
@@ -1885,35 +1902,41 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" s="1"/>
-      <c r="B33" s="1" t="s">
-        <v>82</v>
+      <c r="B33" s="5" t="s">
+        <v>76</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="D33" s="2">
-        <v>128.05000000000001</v>
-      </c>
-      <c r="E33" s="3">
-        <v>16470</v>
-      </c>
-      <c r="F33" s="4"/>
-      <c r="G33" s="4"/>
-      <c r="H33" s="4"/>
+        <v>102.23</v>
+      </c>
+      <c r="E33" s="3"/>
+      <c r="F33" s="3">
+        <f>+[10]Main!$K$5-[10]Main!$K$6</f>
+        <v>3155</v>
+      </c>
+      <c r="G33" s="3">
+        <f>E33-F33</f>
+        <v>-3155</v>
+      </c>
+      <c r="H33" s="4" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" s="1"/>
       <c r="B34" s="1" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="D34" s="2">
-        <v>63.5</v>
+        <v>40.44</v>
       </c>
       <c r="E34" s="3">
-        <v>16440</v>
+        <v>16810</v>
       </c>
       <c r="F34" s="4"/>
       <c r="G34" s="4"/>
@@ -1922,16 +1945,16 @@
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" s="1"/>
       <c r="B35" s="1" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="D35" s="2">
-        <v>363.45</v>
+        <v>128.05000000000001</v>
       </c>
       <c r="E35" s="3">
-        <v>15250</v>
+        <v>16470</v>
       </c>
       <c r="F35" s="4"/>
       <c r="G35" s="4"/>
@@ -1940,16 +1963,16 @@
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" s="1"/>
       <c r="B36" s="1" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="D36" s="2">
-        <v>135.02000000000001</v>
+        <v>63.5</v>
       </c>
       <c r="E36" s="3">
-        <v>14050</v>
+        <v>16440</v>
       </c>
       <c r="F36" s="4"/>
       <c r="G36" s="4"/>
@@ -1958,16 +1981,16 @@
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" s="1"/>
       <c r="B37" s="1" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="D37" s="2">
-        <v>206.61</v>
+        <v>363.45</v>
       </c>
       <c r="E37" s="3">
-        <v>13880</v>
+        <v>15250</v>
       </c>
       <c r="F37" s="4"/>
       <c r="G37" s="4"/>
@@ -1976,13 +1999,17 @@
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" s="1"/>
       <c r="B38" s="1" t="s">
-        <v>150</v>
+        <v>91</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="D38" s="2"/>
-      <c r="E38" s="3"/>
+        <v>92</v>
+      </c>
+      <c r="D38" s="2">
+        <v>135.02000000000001</v>
+      </c>
+      <c r="E38" s="3">
+        <v>14050</v>
+      </c>
       <c r="F38" s="4"/>
       <c r="G38" s="4"/>
       <c r="H38" s="4"/>
@@ -1990,16 +2017,16 @@
     <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" s="1"/>
       <c r="B39" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D39" s="2">
-        <v>115.52</v>
+        <v>206.61</v>
       </c>
       <c r="E39" s="3">
-        <v>13640</v>
+        <v>13880</v>
       </c>
       <c r="F39" s="4"/>
       <c r="G39" s="4"/>
@@ -2008,17 +2035,13 @@
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" s="1"/>
       <c r="B40" s="1" t="s">
-        <v>96</v>
+        <v>150</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="D40" s="2">
-        <v>206.68</v>
-      </c>
-      <c r="E40" s="3">
-        <v>12990</v>
-      </c>
+        <v>151</v>
+      </c>
+      <c r="D40" s="2"/>
+      <c r="E40" s="3"/>
       <c r="F40" s="4"/>
       <c r="G40" s="4"/>
       <c r="H40" s="4"/>
@@ -2026,16 +2049,16 @@
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" s="1"/>
       <c r="B41" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="D41" s="2">
-        <v>43.77</v>
+        <v>115.52</v>
       </c>
       <c r="E41" s="3">
-        <v>12660</v>
+        <v>13640</v>
       </c>
       <c r="F41" s="4"/>
       <c r="G41" s="4"/>
@@ -2044,16 +2067,16 @@
     <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" s="1"/>
       <c r="B42" s="1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="D42" s="2">
-        <v>2.5099999999999998</v>
+        <v>206.68</v>
       </c>
       <c r="E42" s="3">
-        <v>12580</v>
+        <v>12990</v>
       </c>
       <c r="F42" s="4"/>
       <c r="G42" s="4"/>
@@ -2062,16 +2085,16 @@
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" s="1"/>
       <c r="B43" s="1" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="D43" s="2">
-        <v>98.74</v>
+        <v>43.77</v>
       </c>
       <c r="E43" s="3">
-        <v>12490</v>
+        <v>12660</v>
       </c>
       <c r="F43" s="4"/>
       <c r="G43" s="4"/>
@@ -2080,16 +2103,16 @@
     <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" s="1"/>
       <c r="B44" s="1" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="D44" s="2">
-        <v>40.369999999999997</v>
+        <v>2.5099999999999998</v>
       </c>
       <c r="E44" s="3">
-        <v>11000</v>
+        <v>12580</v>
       </c>
       <c r="F44" s="4"/>
       <c r="G44" s="4"/>
@@ -2098,16 +2121,16 @@
     <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45" s="1"/>
       <c r="B45" s="1" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="D45" s="2">
-        <v>408.48</v>
+        <v>98.74</v>
       </c>
       <c r="E45" s="3">
-        <v>10570</v>
+        <v>12490</v>
       </c>
       <c r="F45" s="4"/>
       <c r="G45" s="4"/>
@@ -2116,16 +2139,16 @@
     <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46" s="1"/>
       <c r="B46" s="1" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="D46" s="2">
-        <v>184.44</v>
+        <v>40.369999999999997</v>
       </c>
       <c r="E46" s="3">
-        <v>10400</v>
+        <v>11000</v>
       </c>
       <c r="F46" s="4"/>
       <c r="G46" s="4"/>
@@ -2134,16 +2157,16 @@
     <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" s="1"/>
       <c r="B47" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="D47" s="2">
-        <v>80.52</v>
+        <v>408.48</v>
       </c>
       <c r="E47" s="3">
-        <v>10310</v>
+        <v>10570</v>
       </c>
       <c r="F47" s="4"/>
       <c r="G47" s="4"/>
@@ -2152,16 +2175,16 @@
     <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" s="1"/>
       <c r="B48" s="1" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="D48" s="2">
-        <v>35.200000000000003</v>
+        <v>184.44</v>
       </c>
       <c r="E48" s="3">
-        <v>10210</v>
+        <v>10400</v>
       </c>
       <c r="F48" s="4"/>
       <c r="G48" s="4"/>
@@ -2170,12 +2193,16 @@
     <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" s="1"/>
       <c r="B49" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="C49" s="1"/>
-      <c r="D49" s="2"/>
+        <v>109</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D49" s="2">
+        <v>80.52</v>
+      </c>
       <c r="E49" s="3">
-        <v>10000</v>
+        <v>10310</v>
       </c>
       <c r="F49" s="4"/>
       <c r="G49" s="4"/>
@@ -2184,16 +2211,16 @@
     <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" s="1"/>
       <c r="B50" s="1" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="D50" s="2">
-        <v>8.17</v>
+        <v>35.200000000000003</v>
       </c>
       <c r="E50" s="3">
-        <v>9320</v>
+        <v>10210</v>
       </c>
       <c r="F50" s="4"/>
       <c r="G50" s="4"/>
@@ -2202,16 +2229,12 @@
     <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" s="1"/>
       <c r="B51" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="D51" s="2">
-        <v>14.73</v>
-      </c>
+        <v>113</v>
+      </c>
+      <c r="C51" s="1"/>
+      <c r="D51" s="2"/>
       <c r="E51" s="3">
-        <v>9140</v>
+        <v>10000</v>
       </c>
       <c r="F51" s="4"/>
       <c r="G51" s="4"/>
@@ -2220,16 +2243,16 @@
     <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52" s="1"/>
       <c r="B52" s="1" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="D52" s="2">
-        <v>56.9</v>
+        <v>8.17</v>
       </c>
       <c r="E52" s="3">
-        <v>9000</v>
+        <v>9320</v>
       </c>
       <c r="F52" s="4"/>
       <c r="G52" s="4"/>
@@ -2238,16 +2261,16 @@
     <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" s="1"/>
       <c r="B53" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="D53" s="2">
-        <v>203.42</v>
+        <v>14.73</v>
       </c>
       <c r="E53" s="3">
-        <v>8580</v>
+        <v>9140</v>
       </c>
       <c r="F53" s="4"/>
       <c r="G53" s="4"/>
@@ -2256,16 +2279,16 @@
     <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54" s="1"/>
       <c r="B54" s="1" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="D54" s="2">
-        <v>126.81</v>
+        <v>56.9</v>
       </c>
       <c r="E54" s="3">
-        <v>8200</v>
+        <v>9000</v>
       </c>
       <c r="F54" s="4"/>
       <c r="G54" s="4"/>
@@ -2274,16 +2297,16 @@
     <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55" s="1"/>
       <c r="B55" s="1" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="D55" s="2">
-        <v>50.35</v>
+        <v>203.42</v>
       </c>
       <c r="E55" s="3">
-        <v>8150</v>
+        <v>8580</v>
       </c>
       <c r="F55" s="4"/>
       <c r="G55" s="4"/>
@@ -2292,12 +2315,16 @@
     <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A56" s="1"/>
       <c r="B56" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="C56" s="1"/>
-      <c r="D56" s="2"/>
+        <v>123</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="D56" s="2">
+        <v>126.81</v>
+      </c>
       <c r="E56" s="3">
-        <v>8000</v>
+        <v>8200</v>
       </c>
       <c r="F56" s="4"/>
       <c r="G56" s="4"/>
@@ -2306,16 +2333,16 @@
     <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A57" s="1"/>
       <c r="B57" s="1" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="D57" s="2">
-        <v>88.7</v>
+        <v>50.35</v>
       </c>
       <c r="E57" s="3">
-        <v>7910</v>
+        <v>8150</v>
       </c>
       <c r="F57" s="4"/>
       <c r="G57" s="4"/>
@@ -2324,16 +2351,12 @@
     <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A58" s="1"/>
       <c r="B58" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="C58" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="D58" s="2">
-        <v>78.3</v>
-      </c>
+        <v>127</v>
+      </c>
+      <c r="C58" s="1"/>
+      <c r="D58" s="2"/>
       <c r="E58" s="3">
-        <v>7580</v>
+        <v>8000</v>
       </c>
       <c r="F58" s="4"/>
       <c r="G58" s="4"/>
@@ -2342,16 +2365,16 @@
     <row r="59" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A59" s="1"/>
       <c r="B59" s="1" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="D59" s="2">
-        <v>50.36</v>
+        <v>88.7</v>
       </c>
       <c r="E59" s="3">
-        <v>7140</v>
+        <v>7910</v>
       </c>
       <c r="F59" s="4"/>
       <c r="G59" s="4"/>
@@ -2360,16 +2383,16 @@
     <row r="60" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A60" s="1"/>
       <c r="B60" s="1" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="D60" s="2">
-        <v>80.58</v>
+        <v>78.3</v>
       </c>
       <c r="E60" s="3">
-        <v>6930</v>
+        <v>7580</v>
       </c>
       <c r="F60" s="4"/>
       <c r="G60" s="4"/>
@@ -2378,16 +2401,16 @@
     <row r="61" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A61" s="1"/>
       <c r="B61" s="1" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="D61" s="2">
-        <v>32.869999999999997</v>
+        <v>50.36</v>
       </c>
       <c r="E61" s="3">
-        <v>6880</v>
+        <v>7140</v>
       </c>
       <c r="F61" s="4"/>
       <c r="G61" s="4"/>
@@ -2396,16 +2419,16 @@
     <row r="62" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A62" s="1"/>
       <c r="B62" s="1" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="D62" s="2">
-        <v>54.6</v>
+        <v>80.58</v>
       </c>
       <c r="E62" s="3">
-        <v>6370</v>
+        <v>6930</v>
       </c>
       <c r="F62" s="4"/>
       <c r="G62" s="4"/>
@@ -2414,16 +2437,16 @@
     <row r="63" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A63" s="1"/>
       <c r="B63" s="1" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="D63" s="2">
-        <v>62.59</v>
+        <v>32.869999999999997</v>
       </c>
       <c r="E63" s="3">
-        <v>6350</v>
+        <v>6880</v>
       </c>
       <c r="F63" s="4"/>
       <c r="G63" s="4"/>
@@ -2432,16 +2455,16 @@
     <row r="64" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A64" s="1"/>
       <c r="B64" s="1" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="D64" s="2">
-        <v>62.71</v>
+        <v>54.6</v>
       </c>
       <c r="E64" s="3">
-        <v>3603</v>
+        <v>6370</v>
       </c>
       <c r="F64" s="4"/>
       <c r="G64" s="4"/>
@@ -2450,16 +2473,16 @@
     <row r="65" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A65" s="1"/>
       <c r="B65" s="1" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="D65" s="2">
-        <v>21.19</v>
+        <v>62.59</v>
       </c>
       <c r="E65" s="3">
-        <v>2965</v>
+        <v>6350</v>
       </c>
       <c r="F65" s="4"/>
       <c r="G65" s="4"/>
@@ -2468,24 +2491,68 @@
     <row r="66" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A66" s="1"/>
       <c r="B66" s="1" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="D66" s="2">
-        <v>26.99</v>
+        <v>62.71</v>
       </c>
       <c r="E66" s="3">
-        <v>1400</v>
+        <v>3603</v>
       </c>
       <c r="F66" s="4"/>
       <c r="G66" s="4"/>
       <c r="H66" s="4"/>
     </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A67" s="1"/>
+      <c r="B67" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="D67" s="2">
+        <v>21.19</v>
+      </c>
+      <c r="E67" s="3">
+        <v>2965</v>
+      </c>
+      <c r="F67" s="4"/>
+      <c r="G67" s="4"/>
+      <c r="H67" s="4"/>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A68" s="1"/>
+      <c r="B68" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="D68" s="2">
+        <v>26.99</v>
+      </c>
+      <c r="E68" s="3">
+        <v>1400</v>
+      </c>
+      <c r="F68" s="4"/>
+      <c r="G68" s="4"/>
+      <c r="H68" s="4"/>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B69" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>155</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B31" r:id="rId1" xr:uid="{97435930-C626-477E-A356-37C8034EEA13}"/>
+    <hyperlink ref="B33" r:id="rId1" xr:uid="{97435930-C626-477E-A356-37C8034EEA13}"/>
     <hyperlink ref="B9" r:id="rId2" xr:uid="{6B983B96-90EF-44CE-83F9-BAD81EABD2D5}"/>
     <hyperlink ref="B7" r:id="rId3" xr:uid="{BD7039C2-9BDE-4B67-88B5-46FD7943C86D}"/>
     <hyperlink ref="B10" r:id="rId4" xr:uid="{7ABE68B7-B1CC-4C84-89C3-1AB7B9FBFA97}"/>
@@ -2501,6 +2568,58 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1944D1A1-17CE-46E2-8476-8B81B74D84F5}">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>162</v>
+      </c>
+      <c r="C3" t="s">
+        <v>161</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A1" location="General!A1" display="Main" xr:uid="{CFF362D0-304B-4B7A-B34B-63C5A9CBF050}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2323FDB-FA5E-4B3B-AF9D-A0B42B1C15D6}">
   <dimension ref="A2:H7"/>
   <sheetViews>
@@ -2605,7 +2724,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48438AAB-DA34-44CA-9338-55235D0D16ED}">
   <dimension ref="A2:H5"/>
   <sheetViews>
@@ -2684,7 +2803,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A47DEF4-794E-4338-900B-30040EBA5B50}">
   <dimension ref="A2:H6"/>
   <sheetViews>
@@ -2779,7 +2898,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CB4FD0E-0CB6-41A0-A74F-ACA34F90ACF7}">
   <dimension ref="A2:H8"/>
   <sheetViews>
@@ -2913,7 +3032,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AF8941A-B291-4743-8598-CC93A9617552}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -2925,7 +3044,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E3454FA-DCC7-4BA3-9C12-C651A3A409D0}">
   <dimension ref="B3:C3"/>
   <sheetViews>

</xml_diff>

<commit_message>
new trading account updates
</commit_message>
<xml_diff>
--- a/Software.xlsx
+++ b/Software.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr filterPrivacy="1" showInkAnnotation="0" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4FD105E-EAEA-483E-849A-EE7F3D9266D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{784CB355-0F40-474F-A84F-39E28E0EC3B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="52245" yWindow="180" windowWidth="24495" windowHeight="20445" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="78045" yWindow="1050" windowWidth="25035" windowHeight="19590" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -116,7 +116,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="577" uniqueCount="325">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="577" uniqueCount="326">
   <si>
     <t>Name</t>
   </si>
@@ -1091,6 +1091,9 @@
   </si>
   <si>
     <t>AMS SM</t>
+  </si>
+  <si>
+    <t>MA</t>
   </si>
 </sst>
 </file>
@@ -1100,13 +1103,19 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0\x"/>
   </numFmts>
-  <fonts count="50" x14ac:knownFonts="1">
+  <fonts count="51" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -1492,234 +1501,235 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="115">
+  <cellXfs count="116">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="43" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="44" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="3" fontId="44" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="3" fontId="43" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="3" fontId="42" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="47" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="3" fontId="46" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="38" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="37" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="38" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="3" fontId="37" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="38" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="38" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="37" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="37" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="4" fontId="38" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="38" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="38" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="38" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="38" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="38" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="38" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="37" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="37" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="37" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="37" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="37" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="37" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="37" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="36" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="38" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="9" fontId="35" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="37" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="4" fontId="38" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="14" fontId="38" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="4" fontId="37" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="14" fontId="37" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="41" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="40" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="3" fontId="44" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="47" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="28" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="4" fontId="44" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="4" fontId="47" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="3" fontId="43" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="3" fontId="46" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="3" fontId="27" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="4" fontId="43" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="48" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="4" fontId="46" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="41" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="47" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="41" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="14" fontId="40" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="41" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="4" fontId="40" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="24" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="3" fontId="40" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="24" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="3" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="23" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="3" fontId="23" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="3" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="3" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="3" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="3" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="3" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="3" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="49" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="48" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="50" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="49" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="3" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="14" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="3" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="3" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -3116,11 +3126,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EE865A7-531A-484D-A1B8-5616406C41D1}">
   <dimension ref="A2:X66"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+    <sheetView zoomScale="190" zoomScaleNormal="190" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <pane xSplit="3" ySplit="3" topLeftCell="D4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A30" sqref="A30"/>
-      <selection pane="bottomRight" activeCell="D18" sqref="D18"/>
+      <selection pane="bottomRight" activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5610,18 +5620,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDDC990C-C1C5-4FE2-B554-717099EBE596}">
   <dimension ref="A1:X24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C3" sqref="C3"/>
+      <selection pane="bottomRight" activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="5" style="10" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.7109375" style="10" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="10"/>
+    <col min="3" max="9" width="9.140625" style="10"/>
+    <col min="10" max="10" width="10.28515625" style="10" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="10"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24" x14ac:dyDescent="0.2">
@@ -5774,11 +5786,11 @@
         <v>20</v>
       </c>
       <c r="D5" s="21">
-        <v>393.84</v>
+        <v>309.18</v>
       </c>
       <c r="E5" s="22">
         <f>+D5*[27]Main!$N$3</f>
-        <v>186089.4</v>
+        <v>146087.55000000002</v>
       </c>
       <c r="F5" s="22">
         <f>+[27]Main!$N$5-[27]Main!$N$6</f>
@@ -5786,13 +5798,18 @@
       </c>
       <c r="G5" s="22">
         <f t="shared" ref="G5" si="0">+E5-F5</f>
-        <v>184916.4</v>
-      </c>
-      <c r="H5" s="22"/>
+        <v>144914.55000000002</v>
+      </c>
+      <c r="H5" s="22">
+        <f>+[27]Main!$N$3</f>
+        <v>472.5</v>
+      </c>
       <c r="I5" s="23" t="s">
         <v>210</v>
       </c>
-      <c r="J5" s="23"/>
+      <c r="J5" s="45">
+        <v>44819</v>
+      </c>
       <c r="K5" s="24"/>
       <c r="L5" s="24"/>
       <c r="M5" s="24"/>
@@ -6221,7 +6238,7 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B17" sqref="B17"/>
+      <selection pane="bottomRight" activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -6337,8 +6354,8 @@
       <c r="B4" s="54" t="s">
         <v>170</v>
       </c>
-      <c r="C4" s="54" t="s">
-        <v>3</v>
+      <c r="C4" s="115" t="s">
+        <v>325</v>
       </c>
       <c r="D4" s="71">
         <v>340.89</v>
@@ -6716,7 +6733,7 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D19" sqref="D19"/>
+      <selection pane="bottomRight" activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -7202,7 +7219,7 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D6" sqref="D6"/>
+      <selection pane="bottomRight" activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
updates from work desktop
</commit_message>
<xml_diff>
--- a/Software.xlsx
+++ b/Software.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr filterPrivacy="1" showInkAnnotation="0" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B0A9552-BA41-4F32-9F8C-A6F5BB043C38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FD1C7AB-BF21-4714-A6DA-2AB529884B2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-32070" yWindow="1665" windowWidth="29520" windowHeight="18420" firstSheet="1" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="16250" yWindow="900" windowWidth="19120" windowHeight="19600" firstSheet="2" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Acquisitions" sheetId="18" r:id="rId1"/>
@@ -4885,18 +4885,18 @@
     <sheetDataSet>
       <sheetData sheetId="0">
         <row r="3">
-          <cell r="K3">
-            <v>1822.306223</v>
+          <cell r="L3">
+            <v>130.81787600000001</v>
           </cell>
         </row>
         <row r="5">
-          <cell r="K5">
-            <v>21277</v>
+          <cell r="L5">
+            <v>585.51599999999996</v>
           </cell>
         </row>
         <row r="6">
-          <cell r="K6">
-            <v>20602</v>
+          <cell r="L6">
+            <v>0</v>
           </cell>
         </row>
       </sheetData>
@@ -4914,23 +4914,23 @@
     </xxl21:alternateUrls>
     <sheetNames>
       <sheetName val="Main"/>
-      <sheetName val="Models"/>
+      <sheetName val="Model"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0">
         <row r="3">
-          <cell r="L3">
-            <v>280</v>
+          <cell r="K3">
+            <v>1822.306223</v>
           </cell>
         </row>
         <row r="5">
-          <cell r="L5">
-            <v>4205</v>
+          <cell r="K5">
+            <v>21277</v>
           </cell>
         </row>
         <row r="6">
-          <cell r="L6">
-            <v>6038</v>
+          <cell r="K6">
+            <v>20602</v>
           </cell>
         </row>
       </sheetData>
@@ -4948,23 +4948,23 @@
     </xxl21:alternateUrls>
     <sheetNames>
       <sheetName val="Main"/>
-      <sheetName val="Model"/>
+      <sheetName val="Models"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0">
         <row r="3">
-          <cell r="M3">
-            <v>1047</v>
+          <cell r="L3">
+            <v>280</v>
           </cell>
         </row>
         <row r="5">
-          <cell r="M5">
-            <v>18269</v>
+          <cell r="L5">
+            <v>4205</v>
           </cell>
         </row>
         <row r="6">
-          <cell r="M6">
-            <v>9727</v>
+          <cell r="L6">
+            <v>6038</v>
           </cell>
         </row>
       </sheetData>
@@ -5017,28 +5017,26 @@
     <sheetNames>
       <sheetName val="Main"/>
       <sheetName val="Model"/>
-      <sheetName val="Brokers"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0">
         <row r="3">
-          <cell r="L3">
-            <v>884.55399999999997</v>
+          <cell r="M3">
+            <v>1047</v>
           </cell>
         </row>
         <row r="5">
-          <cell r="L5">
-            <v>7251</v>
+          <cell r="M5">
+            <v>18269</v>
           </cell>
         </row>
         <row r="6">
-          <cell r="L6">
-            <v>0</v>
+          <cell r="M6">
+            <v>9727</v>
           </cell>
         </row>
       </sheetData>
       <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -5053,29 +5051,28 @@
     <sheetNames>
       <sheetName val="Main"/>
       <sheetName val="Model"/>
+      <sheetName val="Brokers"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0">
         <row r="3">
           <cell r="L3">
-            <v>2449.375</v>
-          </cell>
-          <cell r="O3">
-            <v>19595</v>
+            <v>884.55399999999997</v>
           </cell>
         </row>
         <row r="5">
-          <cell r="O5">
-            <v>1029873</v>
+          <cell r="L5">
+            <v>7251</v>
           </cell>
         </row>
         <row r="6">
-          <cell r="O6">
-            <v>207937</v>
+          <cell r="L6">
+            <v>0</v>
           </cell>
         </row>
       </sheetData>
       <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -5095,17 +5092,20 @@
       <sheetData sheetId="0">
         <row r="3">
           <cell r="L3">
-            <v>633.17718300000001</v>
+            <v>2449.375</v>
+          </cell>
+          <cell r="O3">
+            <v>19595</v>
           </cell>
         </row>
         <row r="5">
-          <cell r="L5">
-            <v>9629.1059999999998</v>
+          <cell r="O5">
+            <v>1029873</v>
           </cell>
         </row>
         <row r="6">
-          <cell r="L6">
-            <v>1985.6590000000001</v>
+          <cell r="O6">
+            <v>207937</v>
           </cell>
         </row>
       </sheetData>
@@ -5116,37 +5116,6 @@
 </file>
 
 <file path=xl/externalLinks/externalLink53.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Main"/>
-      <sheetName val="Model"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="3">
-          <cell r="M3">
-            <v>1260</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="M5">
-            <v>7246.6900000000005</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="M6">
-            <v>911.54899999999998</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink54.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <xxl21:alternateUrls>
@@ -5159,18 +5128,49 @@
     <sheetDataSet>
       <sheetData sheetId="0">
         <row r="3">
-          <cell r="K3">
-            <v>108.748718</v>
+          <cell r="L3">
+            <v>633.17718300000001</v>
           </cell>
         </row>
         <row r="5">
-          <cell r="K5">
-            <v>555.70900000000006</v>
+          <cell r="L5">
+            <v>9629.1059999999998</v>
           </cell>
         </row>
         <row r="6">
-          <cell r="K6">
-            <v>1719</v>
+          <cell r="L6">
+            <v>1985.6590000000001</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink54.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Main"/>
+      <sheetName val="Model"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="3">
+          <cell r="M3">
+            <v>1260</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="M5">
+            <v>7246.6900000000005</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="M6">
+            <v>911.54899999999998</v>
           </cell>
         </row>
       </sheetData>
@@ -5194,17 +5194,17 @@
       <sheetData sheetId="0">
         <row r="3">
           <cell r="K3">
-            <v>103.66987899999999</v>
+            <v>108.748718</v>
           </cell>
         </row>
         <row r="5">
           <cell r="K5">
-            <v>605.38900000000001</v>
+            <v>555.70900000000006</v>
           </cell>
         </row>
         <row r="6">
           <cell r="K6">
-            <v>600.91700000000003</v>
+            <v>1719</v>
           </cell>
         </row>
       </sheetData>
@@ -5227,18 +5227,18 @@
     <sheetDataSet>
       <sheetData sheetId="0">
         <row r="3">
-          <cell r="J3">
-            <v>112.608847</v>
+          <cell r="K3">
+            <v>103.66987899999999</v>
           </cell>
         </row>
         <row r="5">
-          <cell r="J5">
-            <v>69.837999999999994</v>
+          <cell r="K5">
+            <v>605.38900000000001</v>
           </cell>
         </row>
         <row r="6">
-          <cell r="J6">
-            <v>0</v>
+          <cell r="K6">
+            <v>600.91700000000003</v>
           </cell>
         </row>
       </sheetData>
@@ -5261,18 +5261,18 @@
     <sheetDataSet>
       <sheetData sheetId="0">
         <row r="3">
-          <cell r="N3">
-            <v>341.70273399999996</v>
+          <cell r="J3">
+            <v>112.608847</v>
           </cell>
         </row>
         <row r="5">
-          <cell r="N5">
-            <v>1757.3970000000002</v>
+          <cell r="J5">
+            <v>69.837999999999994</v>
           </cell>
         </row>
         <row r="6">
-          <cell r="N6">
-            <v>1285.3420000000001</v>
+          <cell r="J6">
+            <v>0</v>
           </cell>
         </row>
       </sheetData>
@@ -5295,18 +5295,18 @@
     <sheetDataSet>
       <sheetData sheetId="0">
         <row r="3">
-          <cell r="L3">
-            <v>130.81787600000001</v>
+          <cell r="N3">
+            <v>341.70273399999996</v>
           </cell>
         </row>
         <row r="5">
-          <cell r="L5">
-            <v>585.51599999999996</v>
+          <cell r="N5">
+            <v>1757.3970000000002</v>
           </cell>
         </row>
         <row r="6">
-          <cell r="L6">
-            <v>0</v>
+          <cell r="N6">
+            <v>1285.3420000000001</v>
           </cell>
         </row>
       </sheetData>
@@ -5801,24 +5801,24 @@
       <selection pane="bottomRight" activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.42578125" style="147" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.28515625" style="147" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="147"/>
+    <col min="1" max="1" width="5.453125" style="147" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.26953125" style="147" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.1796875" style="147"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="147" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D2" s="147" t="s">
         <v>450</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B3" s="147" t="s">
         <v>454</v>
       </c>
@@ -5826,7 +5826,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B4" s="147" t="s">
         <v>455</v>
       </c>
@@ -5834,7 +5834,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B5" s="147" t="s">
         <v>414</v>
       </c>
@@ -5842,7 +5842,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B6" s="147" t="s">
         <v>457</v>
       </c>
@@ -5850,7 +5850,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B7" s="147" t="s">
         <v>458</v>
       </c>
@@ -5858,7 +5858,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B8" s="147" t="s">
         <v>459</v>
       </c>
@@ -5869,7 +5869,7 @@
         <v>1999</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B9" s="147" t="s">
         <v>461</v>
       </c>
@@ -5877,7 +5877,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B10" s="150" t="s">
         <v>482</v>
       </c>
@@ -5888,7 +5888,7 @@
         <v>1994</v>
       </c>
     </row>
-    <row r="11" spans="1:10" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="69"/>
       <c r="B11" s="5" t="s">
         <v>169</v>
@@ -5934,31 +5934,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDDC990C-C1C5-4FE2-B554-717099EBE596}">
   <dimension ref="A1:AA43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
       <selection pane="bottomRight" activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5" style="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.7109375" style="10" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" style="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.7265625" style="10" customWidth="1"/>
+    <col min="3" max="3" width="12.1796875" style="10" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10" style="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.85546875" style="10" customWidth="1"/>
-    <col min="6" max="9" width="9.140625" style="10"/>
-    <col min="10" max="10" width="10.28515625" style="10" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="10"/>
+    <col min="5" max="5" width="9.81640625" style="10" customWidth="1"/>
+    <col min="6" max="9" width="9.1796875" style="10"/>
+    <col min="10" max="10" width="10.26953125" style="10" customWidth="1"/>
+    <col min="11" max="16384" width="9.1796875" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B2" s="13" t="s">
         <v>0</v>
       </c>
@@ -6032,7 +6032,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3" s="151" t="s">
         <v>253</v>
       </c>
@@ -6075,7 +6075,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A4" s="57"/>
       <c r="B4" s="5" t="s">
         <v>15</v>
@@ -6104,7 +6104,7 @@
       </c>
       <c r="M4" s="178"/>
     </row>
-    <row r="5" spans="1:27" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:27" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="151" t="s">
         <v>253</v>
       </c>
@@ -6165,7 +6165,7 @@
         <v>1982</v>
       </c>
     </row>
-    <row r="6" spans="1:27" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:27" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="67"/>
       <c r="B6" s="5" t="s">
         <v>259</v>
@@ -6212,7 +6212,7 @@
       <c r="V6" s="24"/>
       <c r="W6" s="24"/>
     </row>
-    <row r="7" spans="1:27" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:27" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="118"/>
       <c r="B7" s="5" t="s">
         <v>259</v>
@@ -6259,7 +6259,7 @@
       <c r="V7" s="24"/>
       <c r="W7" s="24"/>
     </row>
-    <row r="8" spans="1:27" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:27" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="68"/>
       <c r="B8" s="68" t="s">
         <v>263</v>
@@ -6295,7 +6295,7 @@
       <c r="V8" s="24"/>
       <c r="W8" s="24"/>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A9" s="69"/>
       <c r="B9" s="10" t="s">
         <v>171</v>
@@ -6311,7 +6311,7 @@
         <v>50938.435697071494</v>
       </c>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A10" s="70"/>
       <c r="B10" s="70" t="s">
         <v>266</v>
@@ -6326,7 +6326,7 @@
         <v>52220</v>
       </c>
     </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A11" s="77"/>
       <c r="B11" s="77" t="s">
         <v>284</v>
@@ -6341,7 +6341,7 @@
         <v>56400</v>
       </c>
     </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A12" s="77"/>
       <c r="B12" s="5" t="s">
         <v>165</v>
@@ -6378,7 +6378,7 @@
         <v>1982</v>
       </c>
     </row>
-    <row r="13" spans="1:27" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:27" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B13" s="5" t="s">
         <v>76</v>
       </c>
@@ -6421,7 +6421,7 @@
         <v>361.68504391428576</v>
       </c>
     </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A14" s="69"/>
       <c r="B14" s="5" t="s">
         <v>653</v>
@@ -6455,7 +6455,7 @@
         <v>45587</v>
       </c>
     </row>
-    <row r="15" spans="1:27" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:27" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B15" s="104" t="s">
         <v>330</v>
       </c>
@@ -6469,7 +6469,7 @@
       <c r="H15" s="4"/>
       <c r="I15" s="4"/>
     </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B16" s="10" t="s">
         <v>167</v>
       </c>
@@ -6483,7 +6483,7 @@
         <v>21290</v>
       </c>
     </row>
-    <row r="17" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>253</v>
       </c>
@@ -6503,7 +6503,7 @@
       <c r="G17" s="4"/>
       <c r="H17" s="4"/>
     </row>
-    <row r="18" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
         <v>467</v>
       </c>
@@ -6516,7 +6516,7 @@
       <c r="G18" s="4"/>
       <c r="H18" s="4"/>
     </row>
-    <row r="19" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
         <v>473</v>
       </c>
@@ -6526,7 +6526,7 @@
       <c r="G19" s="4"/>
       <c r="H19" s="4"/>
     </row>
-    <row r="20" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B20" s="1" t="s">
         <v>475</v>
       </c>
@@ -6539,7 +6539,7 @@
       <c r="G20" s="4"/>
       <c r="H20" s="4"/>
     </row>
-    <row r="21" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
         <v>251</v>
       </c>
@@ -6552,7 +6552,7 @@
       <c r="G21" s="4"/>
       <c r="H21" s="4"/>
     </row>
-    <row r="22" spans="1:26" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:26" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B22" s="87" t="s">
         <v>74</v>
       </c>
@@ -6593,7 +6593,7 @@
       <c r="V22" s="24"/>
       <c r="W22" s="26"/>
     </row>
-    <row r="23" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B23" s="5" t="s">
         <v>655</v>
       </c>
@@ -6608,7 +6608,7 @@
         <v>1641.7643438000002</v>
       </c>
       <c r="F23" s="3">
-        <f>+[58]Main!$L$5-[58]Main!$L$6</f>
+        <f>+[47]Main!$L$5-[47]Main!$L$6</f>
         <v>585.51599999999996</v>
       </c>
       <c r="G23" s="3">
@@ -6616,7 +6616,7 @@
         <v>1056.2483438000004</v>
       </c>
       <c r="H23" s="3">
-        <f>+[58]Main!$L$3</f>
+        <f>+[47]Main!$L$3</f>
         <v>130.81787600000001</v>
       </c>
       <c r="I23" s="4" t="s">
@@ -6626,7 +6626,7 @@
         <v>45629</v>
       </c>
     </row>
-    <row r="24" spans="1:26" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:26" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B24" s="53" t="s">
         <v>250</v>
       </c>
@@ -6651,7 +6651,7 @@
       <c r="V24" s="24"/>
       <c r="W24" s="24"/>
     </row>
-    <row r="25" spans="1:26" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:26" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B25" s="149" t="s">
         <v>479</v>
       </c>
@@ -6679,7 +6679,7 @@
       <c r="V25" s="24"/>
       <c r="W25" s="24"/>
     </row>
-    <row r="26" spans="1:26" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:26" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D26" s="21"/>
       <c r="E26" s="22"/>
       <c r="F26" s="23"/>
@@ -6701,7 +6701,7 @@
       <c r="V26" s="24"/>
       <c r="W26" s="24"/>
     </row>
-    <row r="27" spans="1:26" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:26" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D27" s="21"/>
       <c r="E27" s="22"/>
       <c r="F27" s="23"/>
@@ -6723,7 +6723,7 @@
       <c r="V27" s="24"/>
       <c r="W27" s="24"/>
     </row>
-    <row r="28" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B28" s="1" t="s">
         <v>54</v>
       </c>
@@ -6744,7 +6744,7 @@
         <v>116.66666666666667</v>
       </c>
     </row>
-    <row r="29" spans="1:26" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:26" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B29" s="20" t="s">
         <v>57</v>
       </c>
@@ -6771,7 +6771,7 @@
       <c r="V29" s="24"/>
       <c r="W29" s="24"/>
     </row>
-    <row r="30" spans="1:26" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:26" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B30" s="20" t="s">
         <v>108</v>
       </c>
@@ -6798,22 +6798,22 @@
       <c r="V30" s="24"/>
       <c r="W30" s="24"/>
     </row>
-    <row r="31" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B31" s="51" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="32" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B32" s="125" t="s">
         <v>400</v>
       </c>
     </row>
-    <row r="33" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B33" s="148" t="s">
         <v>463</v>
       </c>
     </row>
-    <row r="34" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B34" s="144" t="s">
         <v>444</v>
       </c>
@@ -6824,7 +6824,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="35" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B35" s="148" t="s">
         <v>464</v>
       </c>
@@ -6833,26 +6833,26 @@
         <v>465</v>
       </c>
     </row>
-    <row r="36" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B36" s="148" t="s">
         <v>469</v>
       </c>
       <c r="H36" s="144"/>
       <c r="J36" s="148"/>
     </row>
-    <row r="37" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B37" s="148" t="s">
         <v>470</v>
       </c>
       <c r="H37" s="144"/>
       <c r="J37" s="148"/>
     </row>
-    <row r="38" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B38" s="148" t="s">
         <v>471</v>
       </c>
     </row>
-    <row r="39" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B39" s="148" t="s">
         <v>477</v>
       </c>
@@ -6860,20 +6860,20 @@
         <v>478</v>
       </c>
     </row>
-    <row r="40" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B40" s="148" t="s">
         <v>472</v>
       </c>
     </row>
-    <row r="41" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B41" s="148" t="s">
         <v>474</v>
       </c>
     </row>
-    <row r="42" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B42" s="148"/>
     </row>
-    <row r="43" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B43" s="148" t="s">
         <v>462</v>
       </c>
@@ -6908,22 +6908,22 @@
       <selection pane="bottomRight" activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5" style="211" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.28515625" style="211" customWidth="1"/>
-    <col min="3" max="3" width="10.42578125" style="211" bestFit="1" customWidth="1"/>
-    <col min="4" max="9" width="9.140625" style="212"/>
-    <col min="10" max="10" width="10.42578125" style="211" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="211"/>
+    <col min="2" max="2" width="18.26953125" style="211" customWidth="1"/>
+    <col min="3" max="3" width="10.453125" style="211" bestFit="1" customWidth="1"/>
+    <col min="4" max="9" width="9.1796875" style="212"/>
+    <col min="10" max="10" width="10.453125" style="211" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.1796875" style="211"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B2" s="213" t="s">
         <v>0</v>
       </c>
@@ -6994,7 +6994,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="3" spans="1:24" s="222" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:24" s="222" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B3" s="138" t="s">
         <v>162</v>
       </c>
@@ -7008,7 +7008,7 @@
         <v>524600</v>
       </c>
       <c r="F3" s="210">
-        <f>+[47]Main!$K$5-[47]Main!$K$6</f>
+        <f>+[48]Main!$K$5-[48]Main!$K$6</f>
         <v>675</v>
       </c>
       <c r="G3" s="210">
@@ -7016,7 +7016,7 @@
         <v>523925</v>
       </c>
       <c r="H3" s="210">
-        <f>+[47]Main!$K$3</f>
+        <f>+[48]Main!$K$3</f>
         <v>1822.306223</v>
       </c>
       <c r="I3" s="241" t="s">
@@ -7026,7 +7026,7 @@
         <v>45575</v>
       </c>
     </row>
-    <row r="4" spans="1:24" s="222" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:24" s="222" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B4" s="222" t="s">
         <v>164</v>
       </c>
@@ -7044,7 +7044,7 @@
       <c r="H4" s="210"/>
       <c r="I4" s="210"/>
     </row>
-    <row r="5" spans="1:24" s="222" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:24" s="222" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B5" s="222" t="s">
         <v>257</v>
       </c>
@@ -7062,7 +7062,7 @@
       <c r="O5" s="211"/>
       <c r="P5" s="211"/>
     </row>
-    <row r="6" spans="1:24" s="222" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:24" s="222" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B6" s="222" t="s">
         <v>261</v>
       </c>
@@ -7080,7 +7080,7 @@
       <c r="O6" s="211"/>
       <c r="P6" s="211"/>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" s="211" t="s">
         <v>253</v>
       </c>
@@ -7098,7 +7098,7 @@
         <v>171640</v>
       </c>
       <c r="F7" s="210">
-        <f>[48]Main!$L$5-[48]Main!$L$6</f>
+        <f>[49]Main!$L$5-[49]Main!$L$6</f>
         <v>-1833</v>
       </c>
       <c r="G7" s="210">
@@ -7106,7 +7106,7 @@
         <v>173473</v>
       </c>
       <c r="H7" s="210">
-        <f>+[48]Main!$L$3</f>
+        <f>+[49]Main!$L$3</f>
         <v>280</v>
       </c>
       <c r="I7" s="233" t="s">
@@ -7130,7 +7130,7 @@
         <v>1984</v>
       </c>
     </row>
-    <row r="8" spans="1:24" s="222" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:24" s="222" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B8" s="138" t="s">
         <v>31</v>
       </c>
@@ -7145,7 +7145,7 @@
         <v>75384</v>
       </c>
       <c r="F8" s="210">
-        <f>[49]Main!$M$5-[49]Main!$M$6</f>
+        <f>[50]Main!$M$5-[50]Main!$M$6</f>
         <v>8542</v>
       </c>
       <c r="G8" s="210">
@@ -7153,7 +7153,7 @@
         <v>66842</v>
       </c>
       <c r="H8" s="210">
-        <f>[49]Main!$M$3</f>
+        <f>[50]Main!$M$3</f>
         <v>1047</v>
       </c>
       <c r="I8" s="210" t="s">
@@ -7165,7 +7165,7 @@
       <c r="O8" s="211"/>
       <c r="P8" s="211"/>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B9" s="211" t="s">
         <v>265</v>
       </c>
@@ -7176,7 +7176,7 @@
         <v>188.13</v>
       </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B10" s="211" t="s">
         <v>268</v>
       </c>
@@ -7187,7 +7187,7 @@
         <v>161.51</v>
       </c>
     </row>
-    <row r="11" spans="1:24" s="222" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:24" s="222" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B11" s="222" t="s">
         <v>243</v>
       </c>
@@ -7207,7 +7207,7 @@
       <c r="O11" s="211"/>
       <c r="P11" s="211"/>
     </row>
-    <row r="12" spans="1:24" s="222" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:24" s="222" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B12" s="222" t="s">
         <v>270</v>
       </c>
@@ -7225,7 +7225,7 @@
       <c r="O12" s="211"/>
       <c r="P12" s="211"/>
     </row>
-    <row r="13" spans="1:24" s="222" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:24" s="222" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B13" s="138" t="s">
         <v>632</v>
       </c>
@@ -7240,7 +7240,7 @@
         <v>20079.375799999998</v>
       </c>
       <c r="F13" s="210">
-        <f>+[50]Main!$L$5-[50]Main!$L$6</f>
+        <f>+[51]Main!$L$5-[51]Main!$L$6</f>
         <v>7251</v>
       </c>
       <c r="G13" s="210">
@@ -7248,7 +7248,7 @@
         <v>12828.375799999998</v>
       </c>
       <c r="H13" s="210">
-        <f>+[50]Main!$L$3</f>
+        <f>+[51]Main!$L$3</f>
         <v>884.55399999999997</v>
       </c>
       <c r="I13" s="210" t="s">
@@ -7260,7 +7260,7 @@
       <c r="O13" s="211"/>
       <c r="P13" s="211"/>
     </row>
-    <row r="14" spans="1:24" s="222" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:24" s="222" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B14" s="222" t="s">
         <v>272</v>
       </c>
@@ -7276,7 +7276,7 @@
       <c r="O14" s="211"/>
       <c r="P14" s="211"/>
     </row>
-    <row r="15" spans="1:24" s="222" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:24" s="222" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B15" s="222" t="s">
         <v>288</v>
       </c>
@@ -7294,7 +7294,7 @@
       <c r="O15" s="211"/>
       <c r="P15" s="211"/>
     </row>
-    <row r="16" spans="1:24" s="222" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:24" s="222" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B16" s="222" t="s">
         <v>289</v>
       </c>
@@ -7312,7 +7312,7 @@
       <c r="O16" s="211"/>
       <c r="P16" s="211"/>
     </row>
-    <row r="17" spans="1:23" s="222" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:23" s="222" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B17" s="222" t="s">
         <v>293</v>
       </c>
@@ -7328,7 +7328,7 @@
       <c r="O17" s="211"/>
       <c r="P17" s="211"/>
     </row>
-    <row r="18" spans="1:23" s="222" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:23" s="222" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B18" s="232" t="s">
         <v>638</v>
       </c>
@@ -7346,7 +7346,7 @@
       <c r="O18" s="211"/>
       <c r="P18" s="211"/>
     </row>
-    <row r="19" spans="1:23" s="222" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:23" s="222" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B19" s="222" t="s">
         <v>296</v>
       </c>
@@ -7364,7 +7364,7 @@
       <c r="O19" s="211"/>
       <c r="P19" s="211"/>
     </row>
-    <row r="20" spans="1:23" s="222" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:23" s="222" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B20" s="222" t="s">
         <v>306</v>
       </c>
@@ -7382,7 +7382,7 @@
       <c r="O20" s="211"/>
       <c r="P20" s="211"/>
     </row>
-    <row r="21" spans="1:23" s="222" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:23" s="222" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B21" s="222" t="s">
         <v>70</v>
       </c>
@@ -7402,7 +7402,7 @@
       <c r="O21" s="211"/>
       <c r="P21" s="211"/>
     </row>
-    <row r="22" spans="1:23" s="222" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:23" s="222" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="222" t="s">
         <v>253</v>
       </c>
@@ -7425,7 +7425,7 @@
       <c r="O22" s="211"/>
       <c r="P22" s="211"/>
     </row>
-    <row r="23" spans="1:23" s="222" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:23" s="222" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="222" t="s">
         <v>253</v>
       </c>
@@ -7448,7 +7448,7 @@
       <c r="O23" s="211"/>
       <c r="P23" s="211"/>
     </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B24" s="229" t="s">
         <v>300</v>
       </c>
@@ -7477,7 +7477,7 @@
       <c r="V24" s="226"/>
       <c r="W24" s="227"/>
     </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A25" s="211" t="s">
         <v>253</v>
       </c>
@@ -7494,7 +7494,7 @@
         <v>19090</v>
       </c>
     </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B26" s="240" t="s">
         <v>645</v>
       </c>
@@ -7508,7 +7508,7 @@
         <v>1700</v>
       </c>
     </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A27" s="211" t="s">
         <v>253</v>
       </c>
@@ -7519,7 +7519,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A28" s="211" t="s">
         <v>253</v>
       </c>
@@ -7530,7 +7530,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A29" s="211" t="s">
         <v>253</v>
       </c>
@@ -7541,7 +7541,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A30" s="211" t="s">
         <v>253</v>
       </c>
@@ -7552,7 +7552,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A31" s="211" t="s">
         <v>253</v>
       </c>
@@ -7563,7 +7563,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A32" s="211" t="s">
         <v>253</v>
       </c>
@@ -7574,7 +7574,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B33" s="245" t="s">
         <v>651</v>
       </c>
@@ -7582,7 +7582,7 @@
         <v>652</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="211" t="s">
         <v>253</v>
       </c>
@@ -7593,7 +7593,7 @@
         <v>588</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="211" t="s">
         <v>253</v>
       </c>
@@ -7604,7 +7604,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="211" t="s">
         <v>253</v>
       </c>
@@ -7615,7 +7615,7 @@
         <v>598</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="211" t="s">
         <v>253</v>
       </c>
@@ -7626,7 +7626,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="211" t="s">
         <v>253</v>
       </c>
@@ -7637,7 +7637,7 @@
         <v>606</v>
       </c>
     </row>
-    <row r="40" spans="1:9" s="222" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:9" s="222" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="B40" s="49" t="s">
         <v>33</v>
       </c>
@@ -7655,7 +7655,7 @@
       <c r="H40" s="210"/>
       <c r="I40" s="210"/>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:9" ht="13" x14ac:dyDescent="0.3">
       <c r="B41" s="126" t="s">
         <v>58</v>
       </c>
@@ -7667,7 +7667,7 @@
         <v>26000</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:9" ht="13" x14ac:dyDescent="0.3">
       <c r="B42" s="222" t="s">
         <v>86</v>
       </c>
@@ -7679,7 +7679,7 @@
         <v>15000</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:9" ht="13" x14ac:dyDescent="0.3">
       <c r="B43" s="211" t="s">
         <v>242</v>
       </c>
@@ -7690,7 +7690,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:9" ht="13" x14ac:dyDescent="0.3">
       <c r="B44" s="211" t="s">
         <v>244</v>
       </c>
@@ -7698,7 +7698,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B45" s="211" t="s">
         <v>274</v>
       </c>
@@ -7706,7 +7706,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B46" s="211" t="s">
         <v>276</v>
       </c>
@@ -7714,7 +7714,7 @@
         <v>159.5</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B47" s="211" t="s">
         <v>401</v>
       </c>
@@ -7743,19 +7743,19 @@
       <selection pane="bottomRight" activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.42578125" style="151" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" style="151" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="151"/>
+    <col min="1" max="1" width="5.453125" style="151" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.453125" style="151" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.1796875" style="151"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" s="151" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B2" s="153" t="s">
         <v>0</v>
       </c>
@@ -7826,7 +7826,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B3" s="152" t="s">
         <v>143</v>
       </c>
@@ -7840,7 +7840,7 @@
         <v>1400</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" s="151" t="s">
         <v>253</v>
       </c>
@@ -7853,7 +7853,7 @@
       <c r="D4" s="162"/>
       <c r="E4" s="163"/>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" s="151" t="s">
         <v>253</v>
       </c>
@@ -7880,21 +7880,21 @@
       <selection pane="bottomRight" activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5" style="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.85546875" style="10" customWidth="1"/>
-    <col min="3" max="9" width="9.140625" style="10"/>
-    <col min="10" max="10" width="10.42578125" style="10" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="10"/>
+    <col min="2" max="2" width="11.81640625" style="10" customWidth="1"/>
+    <col min="3" max="9" width="9.1796875" style="10"/>
+    <col min="10" max="10" width="10.453125" style="10" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.1796875" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="2" spans="1:24" s="57" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:24" s="57" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B2" s="58" t="s">
         <v>0</v>
       </c>
@@ -7965,7 +7965,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" s="170" t="s">
         <v>253</v>
       </c>
@@ -8001,7 +8001,7 @@
         <v>45506</v>
       </c>
     </row>
-    <row r="4" spans="1:24" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:24" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="170" t="s">
         <v>253</v>
       </c>
@@ -8019,7 +8019,7 @@
         <v>233204.99374999999</v>
       </c>
       <c r="F4" s="22" cm="1">
-        <f t="array" ref="F4">([51]Main!$O$5-[51]Main!$O$6)/RMB</f>
+        <f t="array" ref="F4">([52]Main!$O$5-[52]Main!$O$6)/RMB</f>
         <v>121948.96142433234</v>
       </c>
       <c r="G4" s="22">
@@ -8027,7 +8027,7 @@
         <v>111256.03232566765</v>
       </c>
       <c r="H4" s="22">
-        <f>+[51]Main!$L$3</f>
+        <f>+[52]Main!$L$3</f>
         <v>2449.375</v>
       </c>
       <c r="I4" s="192" t="s">
@@ -8050,7 +8050,7 @@
       <c r="V4" s="24"/>
       <c r="W4" s="26"/>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" s="170" t="s">
         <v>253</v>
       </c>
@@ -8068,7 +8068,7 @@
         <v>229654.2587072282</v>
       </c>
       <c r="F5" s="3" cm="1">
-        <f t="array" ref="F5">([51]Main!$O$5-[51]Main!$O$6)/RMB</f>
+        <f t="array" ref="F5">([52]Main!$O$5-[52]Main!$O$6)/RMB</f>
         <v>121948.96142433234</v>
       </c>
       <c r="G5" s="3">
@@ -8076,7 +8076,7 @@
         <v>107705.29728289586</v>
       </c>
       <c r="H5" s="46">
-        <f>+[51]Main!$O$3</f>
+        <f>+[52]Main!$O$3</f>
         <v>19595</v>
       </c>
       <c r="I5" s="4" t="s">
@@ -8087,7 +8087,7 @@
         <v>45559</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" s="67"/>
       <c r="B6" s="1" t="s">
         <v>28</v>
@@ -8102,7 +8102,7 @@
         <v>101795</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" s="67"/>
       <c r="B7" s="67" t="s">
         <v>254</v>
@@ -8111,7 +8111,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" s="170" t="s">
         <v>253</v>
       </c>
@@ -8122,7 +8122,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" s="170" t="s">
         <v>253</v>
       </c>
@@ -8140,7 +8140,7 @@
         <v>73714.487644859997</v>
       </c>
       <c r="F9" s="46">
-        <f>+[52]Main!$L$5-[52]Main!$L$6</f>
+        <f>+[53]Main!$L$5-[53]Main!$L$6</f>
         <v>7643.4470000000001</v>
       </c>
       <c r="G9" s="22">
@@ -8148,7 +8148,7 @@
         <v>66071.040644859997</v>
       </c>
       <c r="H9" s="46">
-        <f>+[52]Main!$L$3</f>
+        <f>+[53]Main!$L$3</f>
         <v>633.17718300000001</v>
       </c>
       <c r="I9" s="116" t="s">
@@ -8158,7 +8158,7 @@
         <v>44971</v>
       </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A10" s="170" t="s">
         <v>253</v>
       </c>
@@ -8169,7 +8169,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A11" s="77"/>
       <c r="B11" s="77" t="s">
         <v>284</v>
@@ -8178,7 +8178,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A12" s="170" t="s">
         <v>253</v>
       </c>
@@ -8189,7 +8189,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="13" spans="1:24" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:24" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="151" t="s">
         <v>253</v>
       </c>
@@ -8203,11 +8203,11 @@
         <v>36.71</v>
       </c>
       <c r="E13" s="22">
-        <f>+D13*[53]Main!$M$3</f>
+        <f>+D13*[54]Main!$M$3</f>
         <v>46254.6</v>
       </c>
       <c r="F13" s="22">
-        <f>+[53]Main!$M$5-[53]Main!$M$6</f>
+        <f>+[54]Main!$M$5-[54]Main!$M$6</f>
         <v>6335.1410000000005</v>
       </c>
       <c r="G13" s="22">
@@ -8233,7 +8233,7 @@
       <c r="V13" s="24"/>
       <c r="W13" s="26"/>
     </row>
-    <row r="14" spans="1:24" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:24" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="77"/>
       <c r="B14" s="77" t="s">
         <v>286</v>
@@ -8262,7 +8262,7 @@
       <c r="V14" s="24"/>
       <c r="W14" s="24"/>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A15" s="84"/>
       <c r="B15" s="1" t="s">
         <v>59</v>
@@ -8277,7 +8277,7 @@
         <v>25171</v>
       </c>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A16" s="84"/>
       <c r="B16" s="84" t="s">
         <v>302</v>
@@ -8286,7 +8286,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A17" s="84"/>
       <c r="B17" s="84" t="s">
         <v>304</v>
@@ -8295,7 +8295,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A18" s="85"/>
       <c r="B18" s="85" t="s">
         <v>308</v>
@@ -8304,7 +8304,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A19" s="86"/>
       <c r="B19" s="86" t="s">
         <v>310</v>
@@ -8313,7 +8313,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A20" s="102"/>
       <c r="B20" s="10" t="s">
         <v>157</v>
@@ -8322,7 +8322,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
         <v>96</v>
       </c>
@@ -8336,7 +8336,7 @@
         <v>12580</v>
       </c>
     </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B22" s="10" t="s">
         <v>159</v>
       </c>
@@ -8344,7 +8344,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="23" spans="1:23" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:23" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B23" s="20" t="s">
         <v>131</v>
       </c>
@@ -8376,7 +8376,7 @@
       <c r="V23" s="24"/>
       <c r="W23" s="26"/>
     </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B24" s="5" t="s">
         <v>377</v>
       </c>
@@ -8391,7 +8391,7 @@
         <v>963.51364147999993</v>
       </c>
       <c r="F24" s="46">
-        <f>+[54]Main!$K$5-[54]Main!$K$6</f>
+        <f>+[55]Main!$K$5-[55]Main!$K$6</f>
         <v>-1163.2909999999999</v>
       </c>
       <c r="G24" s="46">
@@ -8399,7 +8399,7 @@
         <v>2126.8046414800001</v>
       </c>
       <c r="H24" s="46">
-        <f>+[54]Main!$K$3</f>
+        <f>+[55]Main!$K$3</f>
         <v>108.748718</v>
       </c>
       <c r="I24" s="115" t="s">
@@ -8409,7 +8409,7 @@
         <v>44965</v>
       </c>
     </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B25" s="5" t="s">
         <v>630</v>
       </c>
@@ -8424,7 +8424,7 @@
         <v>183.49568582999999</v>
       </c>
       <c r="F25" s="46">
-        <f>+[55]Main!$K$5-[55]Main!$K$6</f>
+        <f>+[56]Main!$K$5-[56]Main!$K$6</f>
         <v>4.47199999999998</v>
       </c>
       <c r="G25" s="46">
@@ -8432,7 +8432,7 @@
         <v>179.02368583000001</v>
       </c>
       <c r="H25" s="46">
-        <f>+[55]Main!$K$3</f>
+        <f>+[56]Main!$K$3</f>
         <v>103.66987899999999</v>
       </c>
       <c r="I25" s="242" t="s">
@@ -8442,12 +8442,12 @@
         <v>45556</v>
       </c>
     </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B26" s="114" t="s">
         <v>379</v>
       </c>
     </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B27" s="5" t="s">
         <v>649</v>
       </c>
@@ -8462,7 +8462,7 @@
         <v>114.86102394</v>
       </c>
       <c r="F27" s="46">
-        <f>+[56]Main!$J$5-[56]Main!$J$6</f>
+        <f>+[57]Main!$J$5-[57]Main!$J$6</f>
         <v>69.837999999999994</v>
       </c>
       <c r="G27" s="10">
@@ -8470,7 +8470,7 @@
         <v>45.023023940000002</v>
       </c>
       <c r="H27" s="46">
-        <f>+[56]Main!$J$3</f>
+        <f>+[57]Main!$J$3</f>
         <v>112.608847</v>
       </c>
       <c r="I27" s="246" t="s">
@@ -8480,7 +8480,7 @@
         <v>45583</v>
       </c>
     </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B28" s="151" t="s">
         <v>510</v>
       </c>
@@ -8488,7 +8488,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B29" s="166" t="s">
         <v>553</v>
       </c>
@@ -8496,7 +8496,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B30" s="166" t="s">
         <v>561</v>
       </c>
@@ -8504,7 +8504,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B31" s="171" t="s">
         <v>615</v>
       </c>
@@ -8512,7 +8512,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B32" s="5" t="s">
         <v>647</v>
       </c>
@@ -8523,7 +8523,7 @@
         <v>41.16</v>
       </c>
     </row>
-    <row r="34" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B34" s="1" t="s">
         <v>115</v>
       </c>
@@ -8533,7 +8533,7 @@
         <v>8333</v>
       </c>
     </row>
-    <row r="35" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B35" s="20" t="s">
         <v>63</v>
       </c>
@@ -8543,7 +8543,7 @@
         <v>22000</v>
       </c>
     </row>
-    <row r="36" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B36" s="20" t="s">
         <v>55</v>
       </c>
@@ -8553,7 +8553,7 @@
         <v>30000</v>
       </c>
     </row>
-    <row r="37" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B37" s="146" t="s">
         <v>451</v>
       </c>
@@ -8590,21 +8590,21 @@
       <selection pane="bottomRight" activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5" style="10" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17" style="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="9" width="9.140625" style="10"/>
-    <col min="10" max="10" width="9.140625" style="55"/>
-    <col min="11" max="16384" width="9.140625" style="10"/>
+    <col min="3" max="9" width="9.1796875" style="10"/>
+    <col min="10" max="10" width="9.1796875" style="55"/>
+    <col min="11" max="16384" width="9.1796875" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B2" s="58" t="s">
         <v>0</v>
       </c>
@@ -8675,7 +8675,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" s="71" t="s">
         <v>253</v>
       </c>
@@ -8686,7 +8686,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" s="151" t="s">
         <v>253</v>
       </c>
@@ -8697,7 +8697,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" s="151" t="s">
         <v>253</v>
       </c>
@@ -8708,7 +8708,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" s="79"/>
       <c r="B6" s="79" t="s">
         <v>291</v>
@@ -8717,7 +8717,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" s="151" t="s">
         <v>253</v>
       </c>
@@ -8734,7 +8734,7 @@
         <v>25220</v>
       </c>
     </row>
-    <row r="8" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>253</v>
       </c>
@@ -8755,7 +8755,7 @@
       <c r="H8" s="4"/>
       <c r="J8" s="4"/>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" s="151" t="s">
         <v>253</v>
       </c>
@@ -8773,7 +8773,7 @@
         <v>28494.590988259999</v>
       </c>
       <c r="F9" s="46">
-        <f>+[57]Main!$N$5-[57]Main!$N$6</f>
+        <f>+[58]Main!$N$5-[58]Main!$N$6</f>
         <v>472.05500000000006</v>
       </c>
       <c r="G9" s="46">
@@ -8781,7 +8781,7 @@
         <v>28022.535988259999</v>
       </c>
       <c r="H9" s="46">
-        <f>+[57]Main!$N$3</f>
+        <f>+[58]Main!$N$3</f>
         <v>341.70273399999996</v>
       </c>
       <c r="I9" s="204" t="s">
@@ -8791,7 +8791,7 @@
         <v>45561</v>
       </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A10" s="151" t="s">
         <v>253</v>
       </c>
@@ -8802,7 +8802,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A11" s="151" t="s">
         <v>253</v>
       </c>
@@ -8813,7 +8813,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A12" s="151" t="s">
         <v>253</v>
       </c>
@@ -8824,7 +8824,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A13" s="151" t="s">
         <v>253</v>
       </c>
@@ -8835,7 +8835,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A14" s="151" t="s">
         <v>253</v>
       </c>
@@ -8846,7 +8846,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A15" s="166" t="s">
         <v>253</v>
       </c>
@@ -8857,7 +8857,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A16" s="166" t="s">
         <v>253</v>
       </c>
@@ -8868,7 +8868,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="166" t="s">
         <v>253</v>
       </c>
@@ -8897,18 +8897,18 @@
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5" style="40" bestFit="1" customWidth="1"/>
-    <col min="2" max="16384" width="9.140625" style="40"/>
+    <col min="2" max="16384" width="9.1796875" style="40"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B2" s="40" t="s">
         <v>146</v>
       </c>
@@ -8916,7 +8916,7 @@
         <v>7.8498000000000001</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B3" s="40" t="s">
         <v>147</v>
       </c>
@@ -8924,7 +8924,7 @@
         <v>6.74</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B4" s="40" t="s">
         <v>207</v>
       </c>
@@ -8932,7 +8932,7 @@
         <v>1.01</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B5" s="40" t="s">
         <v>225</v>
       </c>
@@ -8940,7 +8940,7 @@
         <v>10.54</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B6" s="41" t="s">
         <v>233</v>
       </c>
@@ -8948,7 +8948,7 @@
         <v>136.93</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B7" s="41" t="s">
         <v>234</v>
       </c>
@@ -8976,20 +8976,20 @@
       <selection pane="bottomRight" activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="7"/>
-    <col min="4" max="16384" width="9.140625" style="6"/>
+    <col min="2" max="2" width="19.7265625" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.1796875" style="7"/>
+    <col min="4" max="16384" width="9.1796875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B2" s="6" t="s">
         <v>0</v>
       </c>
@@ -9009,7 +9009,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B3" s="8" t="s">
         <v>33</v>
       </c>
@@ -9020,7 +9020,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B4" s="6" t="s">
         <v>86</v>
       </c>
@@ -9031,7 +9031,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B5" s="6" t="s">
         <v>120</v>
       </c>
@@ -9042,7 +9042,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B6" s="6" t="s">
         <v>140</v>
       </c>
@@ -9050,7 +9050,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B7" s="6" t="s">
         <v>141</v>
       </c>
@@ -9058,7 +9058,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B8" s="12" t="s">
         <v>201</v>
       </c>
@@ -9066,7 +9066,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B9" s="41" t="s">
         <v>235</v>
       </c>
@@ -9083,7 +9083,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B10" s="47" t="s">
         <v>238</v>
       </c>
@@ -9097,7 +9097,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B11" s="123" t="s">
         <v>389</v>
       </c>
@@ -9125,18 +9125,18 @@
       <selection pane="bottomRight" activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5" style="151" bestFit="1" customWidth="1"/>
-    <col min="2" max="16384" width="8.85546875" style="151"/>
+    <col min="2" max="16384" width="8.81640625" style="151"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B2" s="151" t="s">
         <v>224</v>
       </c>
@@ -9147,7 +9147,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B3" s="151" t="s">
         <v>483</v>
       </c>
@@ -9169,24 +9169,24 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5" style="105" bestFit="1" customWidth="1"/>
-    <col min="2" max="16384" width="9.140625" style="105"/>
+    <col min="2" max="16384" width="9.1796875" style="105"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="5"/>
       <c r="B2" s="105" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B3" s="105" t="s">
         <v>337</v>
       </c>
@@ -9194,7 +9194,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B4" s="105" t="s">
         <v>339</v>
       </c>
@@ -9202,42 +9202,42 @@
         <v>340</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B5" s="105" t="s">
         <v>341</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B6" s="105" t="s">
         <v>334</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B7" s="105" t="s">
         <v>332</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B8" s="105" t="s">
         <v>336</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B9" s="105" t="s">
         <v>333</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B10" s="105" t="s">
         <v>342</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B11" s="105" t="s">
         <v>343</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B12" s="105" t="s">
         <v>335</v>
       </c>
@@ -9262,19 +9262,19 @@
       <selection pane="bottomRight" activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5" style="132" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" style="132" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="132"/>
+    <col min="2" max="2" width="12.7265625" style="132" customWidth="1"/>
+    <col min="3" max="16384" width="9.1796875" style="132"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B2" s="132" t="s">
         <v>0</v>
       </c>
@@ -9330,7 +9330,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B3" s="136" t="s">
         <v>417</v>
       </c>
@@ -9387,7 +9387,7 @@
         <v>825015.8</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B5" s="132" t="s">
         <v>9</v>
       </c>
@@ -9425,7 +9425,7 @@
         <v>282836</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B6" s="132" t="s">
         <v>7</v>
       </c>
@@ -9469,7 +9469,7 @@
         <v>204094</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B7" s="132" t="s">
         <v>13</v>
       </c>
@@ -9504,7 +9504,7 @@
         <v>116609</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B8" s="132" t="s">
         <v>405</v>
       </c>
@@ -9536,7 +9536,7 @@
         <v>80096</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B9" s="132" t="s">
         <v>23</v>
       </c>
@@ -9562,7 +9562,7 @@
         <v>46073</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B10" s="132" t="s">
         <v>25</v>
       </c>
@@ -9574,7 +9574,7 @@
         <v>30627.300000000003</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B11" s="132" t="s">
         <v>21</v>
       </c>
@@ -9582,7 +9582,7 @@
         <v>30294</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B12" s="132" t="s">
         <v>19</v>
       </c>
@@ -9594,7 +9594,7 @@
         <v>17363.5</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B13" s="132" t="s">
         <v>406</v>
       </c>
@@ -9617,32 +9617,32 @@
         <v>9401</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B14" s="132" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B15" s="132" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B16" s="132" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="17" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B17" s="132" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="18" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B18" s="132" t="s">
         <v>407</v>
       </c>
     </row>
-    <row r="19" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B19" s="136" t="s">
         <v>174</v>
       </c>
@@ -9662,12 +9662,12 @@
         <v>6622</v>
       </c>
     </row>
-    <row r="20" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B20" s="132" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="21" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B21" s="132" t="s">
         <v>391</v>
       </c>
@@ -9678,22 +9678,22 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="22" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B22" s="132" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="23" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B23" s="132" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="24" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B24" s="132" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="25" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B25" s="132" t="s">
         <v>295</v>
       </c>
@@ -9712,74 +9712,74 @@
   <sheetViews>
     <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5" style="105" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.42578125" style="105" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="105"/>
+    <col min="2" max="2" width="10.453125" style="105" customWidth="1"/>
+    <col min="3" max="16384" width="9.1796875" style="105"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="5"/>
       <c r="B2" s="136" t="s">
         <v>415</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="5"/>
       <c r="B3" s="136" t="s">
         <v>411</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="5"/>
       <c r="B4" s="136" t="s">
         <v>414</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="5"/>
       <c r="B5" s="136" t="s">
         <v>412</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="5"/>
       <c r="B6" s="136" t="s">
         <v>416</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="5"/>
       <c r="B7" s="136" t="s">
         <v>413</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="5"/>
       <c r="B8" s="136"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="5"/>
       <c r="B9" s="136"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="5"/>
       <c r="B10" s="105" t="s">
         <v>348</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B11" s="105" t="s">
         <v>344</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B12" s="105" t="s">
         <v>345</v>
       </c>
@@ -9787,12 +9787,12 @@
         <v>346</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B13" s="105" t="s">
         <v>347</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B14" s="132" t="s">
         <v>408</v>
       </c>
@@ -9800,7 +9800,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B15" s="132" t="s">
         <v>410</v>
       </c>
@@ -9824,26 +9824,26 @@
       <selection pane="bottomRight" activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.453125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.85546875" style="20" customWidth="1"/>
-    <col min="2" max="2" width="16.42578125" style="20" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" style="20" customWidth="1"/>
-    <col min="4" max="4" width="8.7109375" style="21" customWidth="1"/>
-    <col min="5" max="5" width="10.28515625" style="22" customWidth="1"/>
-    <col min="6" max="9" width="9.42578125" style="23" customWidth="1"/>
-    <col min="10" max="10" width="10.42578125" style="23" customWidth="1"/>
-    <col min="11" max="15" width="8.42578125" style="24"/>
-    <col min="16" max="16" width="8.42578125" style="25"/>
-    <col min="17" max="18" width="8.42578125" style="24"/>
-    <col min="19" max="19" width="8.42578125" style="26"/>
-    <col min="20" max="20" width="8.42578125" style="25"/>
-    <col min="21" max="22" width="8.42578125" style="24"/>
-    <col min="23" max="23" width="8.42578125" style="26"/>
-    <col min="24" max="16384" width="8.42578125" style="20"/>
+    <col min="1" max="1" width="4.81640625" style="20" customWidth="1"/>
+    <col min="2" max="2" width="16.453125" style="20" customWidth="1"/>
+    <col min="3" max="3" width="10.7265625" style="20" customWidth="1"/>
+    <col min="4" max="4" width="8.7265625" style="21" customWidth="1"/>
+    <col min="5" max="5" width="10.26953125" style="22" customWidth="1"/>
+    <col min="6" max="9" width="9.453125" style="23" customWidth="1"/>
+    <col min="10" max="10" width="10.453125" style="23" customWidth="1"/>
+    <col min="11" max="15" width="8.453125" style="24"/>
+    <col min="16" max="16" width="8.453125" style="25"/>
+    <col min="17" max="18" width="8.453125" style="24"/>
+    <col min="19" max="19" width="8.453125" style="26"/>
+    <col min="20" max="20" width="8.453125" style="25"/>
+    <col min="21" max="22" width="8.453125" style="24"/>
+    <col min="23" max="23" width="8.453125" style="26"/>
+    <col min="24" max="16384" width="8.453125" style="20"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="L2" s="28">
         <f>AVERAGE(L4:L5)</f>
         <v>-5.0648497352395572E-2</v>
@@ -9865,7 +9865,7 @@
         <v>25.524540294644503</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B3" s="13" t="s">
         <v>0</v>
       </c>
@@ -9936,7 +9936,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" s="151" t="s">
         <v>253</v>
       </c>
@@ -10027,7 +10027,7 @@
         <v>1975</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" s="57"/>
       <c r="B5" s="87" t="s">
         <v>9</v>
@@ -10116,7 +10116,7 @@
         <v>1998</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" s="151" t="s">
         <v>253</v>
       </c>
@@ -10156,7 +10156,7 @@
         <v>1995</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B7" s="91" t="s">
         <v>56</v>
       </c>
@@ -10174,7 +10174,7 @@
         <v>2009</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" s="72"/>
       <c r="B8" s="87" t="s">
         <v>38</v>
@@ -10209,7 +10209,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" s="72"/>
       <c r="B9" s="87" t="s">
         <v>38</v>
@@ -10222,7 +10222,7 @@
       <c r="H9" s="22"/>
       <c r="O9" s="26"/>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A10" s="86"/>
       <c r="B10" s="90" t="s">
         <v>312</v>
@@ -10241,7 +10241,7 @@
         <v>1987</v>
       </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A11" s="151" t="s">
         <v>253</v>
       </c>
@@ -10259,7 +10259,7 @@
       </c>
       <c r="O11" s="26"/>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A12" s="151" t="s">
         <v>253</v>
       </c>
@@ -10278,7 +10278,7 @@
       </c>
       <c r="O12" s="26"/>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B13" s="91" t="s">
         <v>72</v>
       </c>
@@ -10296,7 +10296,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A14" s="151" t="s">
         <v>253</v>
       </c>
@@ -10317,7 +10317,7 @@
         <v>2007</v>
       </c>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A15" s="151" t="s">
         <v>253</v>
       </c>
@@ -10335,7 +10335,7 @@
       </c>
       <c r="O15" s="26"/>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A16" s="151" t="s">
         <v>253</v>
       </c>
@@ -10356,7 +10356,7 @@
         <v>1966</v>
       </c>
     </row>
-    <row r="17" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B17" s="91" t="s">
         <v>101</v>
       </c>
@@ -10371,7 +10371,7 @@
       </c>
       <c r="O17" s="26"/>
     </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B18" s="91" t="s">
         <v>105</v>
       </c>
@@ -10389,7 +10389,7 @@
         <v>2007</v>
       </c>
     </row>
-    <row r="19" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B19" s="91" t="s">
         <v>109</v>
       </c>
@@ -10404,7 +10404,7 @@
       </c>
       <c r="O19" s="26"/>
     </row>
-    <row r="20" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B20" s="91" t="s">
         <v>113</v>
       </c>
@@ -10422,7 +10422,7 @@
         <v>2003</v>
       </c>
     </row>
-    <row r="21" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A21" s="151" t="s">
         <v>253</v>
       </c>
@@ -10440,7 +10440,7 @@
       </c>
       <c r="O21" s="26"/>
     </row>
-    <row r="22" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A22" s="151" t="s">
         <v>253</v>
       </c>
@@ -10458,7 +10458,7 @@
       </c>
       <c r="O22" s="26"/>
     </row>
-    <row r="23" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B23" s="91" t="s">
         <v>121</v>
       </c>
@@ -10473,7 +10473,7 @@
       </c>
       <c r="O23" s="26"/>
     </row>
-    <row r="24" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A24" s="151" t="s">
         <v>253</v>
       </c>
@@ -10491,7 +10491,7 @@
       </c>
       <c r="O24" s="26"/>
     </row>
-    <row r="25" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A25" s="151" t="s">
         <v>253</v>
       </c>
@@ -10509,7 +10509,7 @@
       </c>
       <c r="O25" s="26"/>
     </row>
-    <row r="26" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B26" s="91" t="s">
         <v>133</v>
       </c>
@@ -10524,7 +10524,7 @@
       </c>
       <c r="O26" s="26"/>
     </row>
-    <row r="27" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A27" s="151" t="s">
         <v>253</v>
       </c>
@@ -10542,7 +10542,7 @@
       </c>
       <c r="O27" s="26"/>
     </row>
-    <row r="28" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A28" s="151" t="s">
         <v>253</v>
       </c>
@@ -10560,7 +10560,7 @@
       </c>
       <c r="O28" s="26"/>
     </row>
-    <row r="29" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A29" s="151"/>
       <c r="B29" s="87" t="s">
         <v>333</v>
@@ -10595,7 +10595,7 @@
       </c>
       <c r="O29" s="26"/>
     </row>
-    <row r="30" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A30" s="151" t="s">
         <v>253</v>
       </c>
@@ -10607,7 +10607,7 @@
       </c>
       <c r="O30" s="26"/>
     </row>
-    <row r="31" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A31" s="151" t="s">
         <v>253</v>
       </c>
@@ -10625,7 +10625,7 @@
       </c>
       <c r="O31" s="26"/>
     </row>
-    <row r="32" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B32" s="92" t="s">
         <v>215</v>
       </c>
@@ -10640,7 +10640,7 @@
       </c>
       <c r="O32" s="26"/>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B33" s="92" t="s">
         <v>217</v>
       </c>
@@ -10655,7 +10655,7 @@
       </c>
       <c r="O33" s="26"/>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B34" s="94" t="s">
         <v>226</v>
       </c>
@@ -10664,13 +10664,13 @@
       </c>
       <c r="O34" s="26"/>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B35" s="124" t="s">
         <v>393</v>
       </c>
       <c r="O35" s="26"/>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A36" s="151" t="s">
         <v>253</v>
       </c>
@@ -10682,7 +10682,7 @@
       </c>
       <c r="O36" s="26"/>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A37" s="151" t="s">
         <v>253</v>
       </c>
@@ -10694,7 +10694,7 @@
       </c>
       <c r="O37" s="26"/>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A38" s="151" t="s">
         <v>253</v>
       </c>
@@ -10706,7 +10706,7 @@
       </c>
       <c r="O38" s="26"/>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A39" s="151"/>
       <c r="B39" s="207" t="s">
         <v>637</v>
@@ -10716,7 +10716,7 @@
       </c>
       <c r="O39" s="26"/>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A40" s="151" t="s">
         <v>253</v>
       </c>
@@ -10728,7 +10728,7 @@
       </c>
       <c r="O40" s="26"/>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A41" s="151" t="s">
         <v>253</v>
       </c>
@@ -10740,7 +10740,7 @@
       </c>
       <c r="O41" s="26"/>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A42" s="164" t="s">
         <v>253</v>
       </c>
@@ -10752,7 +10752,7 @@
       </c>
       <c r="O42" s="26"/>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A43" s="166" t="s">
         <v>253</v>
       </c>
@@ -10800,21 +10800,21 @@
       <selection pane="bottomRight" activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5" style="57" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.42578125" style="57" customWidth="1"/>
+    <col min="2" max="2" width="13.453125" style="57" customWidth="1"/>
     <col min="3" max="3" width="11" style="57" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" style="57"/>
+    <col min="4" max="4" width="9.1796875" style="57"/>
     <col min="5" max="5" width="10" style="57" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="57"/>
-    <col min="7" max="7" width="10.140625" style="57" customWidth="1"/>
-    <col min="8" max="9" width="9.140625" style="57"/>
-    <col min="10" max="10" width="10.85546875" style="57" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="57"/>
+    <col min="6" max="6" width="9.1796875" style="57"/>
+    <col min="7" max="7" width="10.1796875" style="57" customWidth="1"/>
+    <col min="8" max="9" width="9.1796875" style="57"/>
+    <col min="10" max="10" width="10.81640625" style="57" customWidth="1"/>
+    <col min="11" max="16384" width="9.1796875" style="57"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>142</v>
       </c>
@@ -10822,7 +10822,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B2" s="58" t="s">
         <v>0</v>
       </c>
@@ -10893,7 +10893,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="3" spans="1:24" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:24" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="57"/>
       <c r="B3" s="87" t="s">
         <v>11</v>
@@ -10982,7 +10982,7 @@
         <v>1994</v>
       </c>
     </row>
-    <row r="4" spans="1:24" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:24" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="151" t="s">
         <v>253</v>
       </c>
@@ -11034,7 +11034,7 @@
         <v>1977</v>
       </c>
     </row>
-    <row r="5" spans="1:24" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:24" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="151" t="s">
         <v>253</v>
       </c>
@@ -11083,7 +11083,7 @@
         <v>1972</v>
       </c>
     </row>
-    <row r="6" spans="1:24" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:24" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="151" t="s">
         <v>253</v>
       </c>
@@ -11149,7 +11149,7 @@
         <v>1999</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" s="67"/>
       <c r="B7" s="5" t="s">
         <v>256</v>
@@ -11186,7 +11186,7 @@
         <v>1911</v>
       </c>
     </row>
-    <row r="8" spans="1:24" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:24" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="151" t="s">
         <v>253</v>
       </c>
@@ -11238,7 +11238,7 @@
         <v>2004</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" s="151" t="s">
         <v>253</v>
       </c>
@@ -11274,7 +11274,7 @@
         <v>45446</v>
       </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A10" s="151" t="s">
         <v>253</v>
       </c>
@@ -11313,7 +11313,7 @@
         <v>2005</v>
       </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A11" s="151" t="s">
         <v>253</v>
       </c>
@@ -11352,7 +11352,7 @@
         <v>2002</v>
       </c>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A12" s="151" t="s">
         <v>253</v>
       </c>
@@ -11391,7 +11391,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A13" s="151" t="s">
         <v>253</v>
       </c>
@@ -11427,7 +11427,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A14" s="151" t="s">
         <v>253</v>
       </c>
@@ -11466,7 +11466,7 @@
         <v>2007</v>
       </c>
     </row>
-    <row r="15" spans="1:24" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:24" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="151" t="s">
         <v>253</v>
       </c>
@@ -11518,7 +11518,7 @@
         <v>2006</v>
       </c>
     </row>
-    <row r="16" spans="1:24" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:24" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="151" t="s">
         <v>253</v>
       </c>
@@ -11570,7 +11570,7 @@
         <v>2007</v>
       </c>
     </row>
-    <row r="17" spans="1:24" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:24" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="151" t="s">
         <v>253</v>
       </c>
@@ -11622,7 +11622,7 @@
         <v>2009</v>
       </c>
     </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A18" s="151" t="s">
         <v>253</v>
       </c>
@@ -11661,7 +11661,7 @@
         <v>2011</v>
       </c>
     </row>
-    <row r="19" spans="1:24" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:24" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="151" t="s">
         <v>253</v>
       </c>
@@ -11699,7 +11699,7 @@
         <v>2003</v>
       </c>
     </row>
-    <row r="20" spans="1:24" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:24" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="151" t="s">
         <v>253</v>
       </c>
@@ -11748,7 +11748,7 @@
       <c r="V20" s="24"/>
       <c r="W20" s="24"/>
     </row>
-    <row r="21" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A21" s="151" t="s">
         <v>253</v>
       </c>
@@ -11768,7 +11768,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="22" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A22" s="151" t="s">
         <v>253</v>
       </c>
@@ -11785,7 +11785,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="23" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B23" s="91" t="s">
         <v>185</v>
       </c>
@@ -11799,7 +11799,7 @@
         <v>17930</v>
       </c>
     </row>
-    <row r="24" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A24" s="151" t="s">
         <v>253</v>
       </c>
@@ -11816,7 +11816,7 @@
         <v>12660</v>
       </c>
     </row>
-    <row r="25" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A25" s="151" t="s">
         <v>253</v>
       </c>
@@ -11833,7 +11833,7 @@
         <v>15070</v>
       </c>
     </row>
-    <row r="26" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A26" s="151" t="s">
         <v>253</v>
       </c>
@@ -11850,7 +11850,7 @@
         <v>12990</v>
       </c>
     </row>
-    <row r="27" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A27" s="151" t="s">
         <v>253</v>
       </c>
@@ -11867,7 +11867,7 @@
         <v>11000</v>
       </c>
     </row>
-    <row r="28" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A28" s="151" t="s">
         <v>253</v>
       </c>
@@ -11885,7 +11885,7 @@
       <c r="I28" s="23"/>
       <c r="J28" s="81"/>
     </row>
-    <row r="29" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A29" s="151" t="s">
         <v>253</v>
       </c>
@@ -11903,7 +11903,7 @@
       <c r="I29" s="80"/>
       <c r="J29" s="81"/>
     </row>
-    <row r="30" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A30" s="151" t="s">
         <v>253</v>
       </c>
@@ -11916,7 +11916,7 @@
       <c r="D30" s="21"/>
       <c r="E30" s="22"/>
     </row>
-    <row r="31" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A31" s="151" t="s">
         <v>253</v>
       </c>
@@ -11929,7 +11929,7 @@
       <c r="D31" s="21"/>
       <c r="E31" s="22"/>
     </row>
-    <row r="32" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A32" s="151" t="s">
         <v>253</v>
       </c>
@@ -11942,7 +11942,7 @@
       <c r="D32" s="21"/>
       <c r="E32" s="22"/>
     </row>
-    <row r="33" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B33" s="91" t="s">
         <v>111</v>
       </c>
@@ -11956,7 +11956,7 @@
         <v>9140</v>
       </c>
     </row>
-    <row r="34" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A34" s="151" t="s">
         <v>253</v>
       </c>
@@ -11969,7 +11969,7 @@
       <c r="D34" s="21"/>
       <c r="E34" s="22"/>
     </row>
-    <row r="35" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A35" s="166" t="s">
         <v>253</v>
       </c>
@@ -11982,7 +11982,7 @@
       <c r="D35" s="21"/>
       <c r="E35" s="22"/>
     </row>
-    <row r="36" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A36" s="151" t="s">
         <v>253</v>
       </c>
@@ -11995,7 +11995,7 @@
       <c r="D36" s="21"/>
       <c r="E36" s="22"/>
     </row>
-    <row r="37" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A37" s="151" t="s">
         <v>253</v>
       </c>
@@ -12012,7 +12012,7 @@
         <v>16020</v>
       </c>
     </row>
-    <row r="38" spans="1:24" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:24" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="151" t="s">
         <v>253</v>
       </c>
@@ -12050,7 +12050,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="39" spans="1:24" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:24" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="151" t="s">
         <v>253</v>
       </c>
@@ -12081,7 +12081,7 @@
       <c r="V39" s="24"/>
       <c r="W39" s="24"/>
     </row>
-    <row r="40" spans="1:24" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:24" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="151" t="s">
         <v>253</v>
       </c>
@@ -12112,7 +12112,7 @@
       <c r="V40" s="24"/>
       <c r="W40" s="24"/>
     </row>
-    <row r="41" spans="1:24" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:24" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="166" t="s">
         <v>253</v>
       </c>
@@ -12161,7 +12161,7 @@
       <c r="V41" s="24"/>
       <c r="W41" s="24"/>
     </row>
-    <row r="42" spans="1:24" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:24" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="166" t="s">
         <v>253</v>
       </c>
@@ -12210,7 +12210,7 @@
       <c r="V42" s="24"/>
       <c r="W42" s="24"/>
     </row>
-    <row r="43" spans="1:24" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:24" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="166" t="s">
         <v>253</v>
       </c>
@@ -12259,7 +12259,7 @@
       <c r="V43" s="24"/>
       <c r="W43" s="24"/>
     </row>
-    <row r="44" spans="1:24" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:24" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="151"/>
       <c r="B44" s="5" t="s">
         <v>617</v>
@@ -12306,7 +12306,7 @@
       <c r="V44" s="24"/>
       <c r="W44" s="24"/>
     </row>
-    <row r="45" spans="1:24" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:24" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="151" t="s">
         <v>253</v>
       </c>
@@ -12337,7 +12337,7 @@
       <c r="V45" s="24"/>
       <c r="W45" s="24"/>
     </row>
-    <row r="46" spans="1:24" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:24" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="151" t="s">
         <v>253</v>
       </c>
@@ -12368,7 +12368,7 @@
       <c r="V46" s="24"/>
       <c r="W46" s="24"/>
     </row>
-    <row r="47" spans="1:24" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:24" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="151" t="s">
         <v>253</v>
       </c>
@@ -12399,7 +12399,7 @@
       <c r="V47" s="24"/>
       <c r="W47" s="24"/>
     </row>
-    <row r="48" spans="1:24" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:24" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="151" t="s">
         <v>253</v>
       </c>
@@ -12430,7 +12430,7 @@
       <c r="V48" s="24"/>
       <c r="W48" s="24"/>
     </row>
-    <row r="49" spans="1:23" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:23" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="151" t="s">
         <v>253</v>
       </c>
@@ -12461,7 +12461,7 @@
       <c r="V49" s="24"/>
       <c r="W49" s="24"/>
     </row>
-    <row r="50" spans="1:23" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:23" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="151" t="s">
         <v>253</v>
       </c>
@@ -12492,7 +12492,7 @@
       <c r="V50" s="24"/>
       <c r="W50" s="24"/>
     </row>
-    <row r="51" spans="1:23" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:23" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="151" t="s">
         <v>253</v>
       </c>
@@ -12523,7 +12523,7 @@
       <c r="V51" s="24"/>
       <c r="W51" s="24"/>
     </row>
-    <row r="52" spans="1:23" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:23" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="151" t="s">
         <v>253</v>
       </c>
@@ -12554,7 +12554,7 @@
       <c r="V52" s="24"/>
       <c r="W52" s="24"/>
     </row>
-    <row r="53" spans="1:23" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:23" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="164" t="s">
         <v>253</v>
       </c>
@@ -12585,7 +12585,7 @@
       <c r="V53" s="24"/>
       <c r="W53" s="24"/>
     </row>
-    <row r="54" spans="1:23" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:23" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="164" t="s">
         <v>253</v>
       </c>
@@ -12616,7 +12616,7 @@
       <c r="V54" s="24"/>
       <c r="W54" s="24"/>
     </row>
-    <row r="55" spans="1:23" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:23" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="166" t="s">
         <v>253</v>
       </c>
@@ -12647,7 +12647,7 @@
       <c r="V55" s="24"/>
       <c r="W55" s="24"/>
     </row>
-    <row r="56" spans="1:23" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:23" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="166" t="s">
         <v>253</v>
       </c>
@@ -12678,7 +12678,7 @@
       <c r="V56" s="24"/>
       <c r="W56" s="24"/>
     </row>
-    <row r="57" spans="1:23" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:23" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="166" t="s">
         <v>253</v>
       </c>
@@ -12709,7 +12709,7 @@
       <c r="V57" s="24"/>
       <c r="W57" s="24"/>
     </row>
-    <row r="58" spans="1:23" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:23" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="166" t="s">
         <v>253</v>
       </c>
@@ -12740,7 +12740,7 @@
       <c r="V58" s="24"/>
       <c r="W58" s="24"/>
     </row>
-    <row r="59" spans="1:23" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:23" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="166" t="s">
         <v>253</v>
       </c>
@@ -12771,7 +12771,7 @@
       <c r="V59" s="24"/>
       <c r="W59" s="24"/>
     </row>
-    <row r="60" spans="1:23" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:23" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="166" t="s">
         <v>253</v>
       </c>
@@ -12802,7 +12802,7 @@
       <c r="V60" s="24"/>
       <c r="W60" s="24"/>
     </row>
-    <row r="61" spans="1:23" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:23" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="166" t="s">
         <v>253</v>
       </c>
@@ -12833,7 +12833,7 @@
       <c r="V61" s="24"/>
       <c r="W61" s="24"/>
     </row>
-    <row r="62" spans="1:23" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:23" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" s="166" t="s">
         <v>253</v>
       </c>
@@ -12864,7 +12864,7 @@
       <c r="V62" s="24"/>
       <c r="W62" s="24"/>
     </row>
-    <row r="63" spans="1:23" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:23" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="166"/>
       <c r="B63" s="5" t="s">
         <v>622</v>
@@ -12898,7 +12898,7 @@
       <c r="V63" s="24"/>
       <c r="W63" s="24"/>
     </row>
-    <row r="64" spans="1:23" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:23" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="166" t="s">
         <v>253</v>
       </c>
@@ -12929,7 +12929,7 @@
       <c r="V64" s="24"/>
       <c r="W64" s="24"/>
     </row>
-    <row r="65" spans="1:23" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:23" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="166" t="s">
         <v>253</v>
       </c>
@@ -12960,7 +12960,7 @@
       <c r="V65" s="24"/>
       <c r="W65" s="24"/>
     </row>
-    <row r="66" spans="1:23" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:23" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="166" t="s">
         <v>253</v>
       </c>
@@ -12991,7 +12991,7 @@
       <c r="V66" s="24"/>
       <c r="W66" s="24"/>
     </row>
-    <row r="67" spans="1:23" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:23" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" s="166" t="s">
         <v>253</v>
       </c>
@@ -13022,7 +13022,7 @@
       <c r="V67" s="24"/>
       <c r="W67" s="24"/>
     </row>
-    <row r="68" spans="1:23" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:23" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A68" s="166" t="s">
         <v>253</v>
       </c>
@@ -13053,7 +13053,7 @@
       <c r="V68" s="24"/>
       <c r="W68" s="24"/>
     </row>
-    <row r="69" spans="1:23" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:23" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A69" s="164"/>
       <c r="B69" s="164"/>
       <c r="C69" s="164"/>
@@ -13078,7 +13078,7 @@
       <c r="V69" s="24"/>
       <c r="W69" s="24"/>
     </row>
-    <row r="70" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:23" ht="13" x14ac:dyDescent="0.3">
       <c r="B70" s="74" t="s">
         <v>248</v>
       </c>
@@ -13086,7 +13086,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="71" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B71" s="125" t="s">
         <v>395</v>
       </c>
@@ -13097,7 +13097,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="72" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B72" s="125" t="s">
         <v>396</v>
       </c>
@@ -13117,7 +13117,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="73" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B73" s="125" t="s">
         <v>120</v>
       </c>
@@ -13128,7 +13128,7 @@
       <c r="G73" s="125"/>
       <c r="H73" s="125"/>
     </row>
-    <row r="74" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B74" s="143" t="s">
         <v>98</v>
       </c>
@@ -13136,7 +13136,7 @@
         <v>12000</v>
       </c>
     </row>
-    <row r="75" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B75" s="73" t="s">
         <v>275</v>
       </c>
@@ -13179,29 +13179,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{494F58CA-3A5E-4A8C-A323-FDAA45D59D23}">
   <dimension ref="A1:Z60"/>
   <sheetViews>
-    <sheetView zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="F13" sqref="F13"/>
+      <selection pane="bottomRight" activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5" style="51" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" style="51" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" style="51" customWidth="1"/>
-    <col min="4" max="9" width="9.140625" style="51"/>
-    <col min="10" max="10" width="10.85546875" style="51" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="51"/>
+    <col min="3" max="3" width="11.7265625" style="51" customWidth="1"/>
+    <col min="4" max="9" width="9.1796875" style="51"/>
+    <col min="10" max="10" width="10.81640625" style="51" customWidth="1"/>
+    <col min="11" max="16384" width="9.1796875" style="51"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B2" s="13" t="s">
         <v>0</v>
       </c>
@@ -13278,7 +13278,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="3" spans="1:26" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:26" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="57"/>
       <c r="B3" s="5" t="s">
         <v>13</v>
@@ -13347,7 +13347,7 @@
         <v>268.30379779527556</v>
       </c>
     </row>
-    <row r="4" spans="1:26" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:26" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="57"/>
       <c r="B4" s="5" t="s">
         <v>15</v>
@@ -13397,7 +13397,7 @@
         <v>1998</v>
       </c>
     </row>
-    <row r="5" spans="1:26" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:26" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="75"/>
       <c r="B5" s="76" t="s">
         <v>280</v>
@@ -13429,7 +13429,7 @@
         <v>2011</v>
       </c>
     </row>
-    <row r="6" spans="1:26" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:26" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="103"/>
       <c r="B6" s="103" t="s">
         <v>328</v>
@@ -13461,7 +13461,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="7" spans="1:26" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:26" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="83"/>
       <c r="B7" s="108" t="s">
         <v>298</v>
@@ -13500,7 +13500,7 @@
         <v>1999</v>
       </c>
     </row>
-    <row r="8" spans="1:26" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:26" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="109"/>
       <c r="B8" s="108" t="s">
         <v>375</v>
@@ -13554,7 +13554,7 @@
         <v>49.784172938666664</v>
       </c>
     </row>
-    <row r="9" spans="1:26" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:26" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B9" s="75" t="s">
         <v>278</v>
       </c>
@@ -13585,7 +13585,7 @@
         <v>2008</v>
       </c>
     </row>
-    <row r="10" spans="1:26" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:26" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B10" s="75" t="s">
         <v>282</v>
       </c>
@@ -13616,7 +13616,7 @@
         <v>2009</v>
       </c>
     </row>
-    <row r="11" spans="1:26" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:26" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B11" s="5" t="s">
         <v>76</v>
       </c>
@@ -13644,7 +13644,7 @@
       <c r="V11" s="24"/>
       <c r="W11" s="24"/>
     </row>
-    <row r="12" spans="1:26" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:26" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B12" s="100" t="s">
         <v>318</v>
       </c>
@@ -13672,7 +13672,7 @@
       <c r="V12" s="24"/>
       <c r="W12" s="24"/>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B13" s="5" t="s">
         <v>321</v>
       </c>
@@ -13705,7 +13705,7 @@
         <v>45601</v>
       </c>
     </row>
-    <row r="14" spans="1:26" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:26" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B14" s="91" t="s">
         <v>129</v>
       </c>
@@ -13713,7 +13713,7 @@
         <v>130</v>
       </c>
       <c r="D14" s="21">
-        <v>32.869999999999997</v>
+        <v>8</v>
       </c>
       <c r="E14" s="22">
         <v>6880</v>
@@ -13737,7 +13737,7 @@
       <c r="V14" s="24"/>
       <c r="W14" s="26"/>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B15" s="100" t="s">
         <v>323</v>
       </c>
@@ -13751,7 +13751,7 @@
         <v>4600</v>
       </c>
     </row>
-    <row r="16" spans="1:26" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:26" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B16" s="5" t="s">
         <v>358</v>
       </c>
@@ -13800,7 +13800,7 @@
         <v>2009</v>
       </c>
     </row>
-    <row r="17" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B17" s="5" t="s">
         <v>641</v>
       </c>
@@ -13833,7 +13833,7 @@
         <v>45575</v>
       </c>
     </row>
-    <row r="18" spans="2:23" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:23" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B18" s="175" t="s">
         <v>619</v>
       </c>
@@ -13859,7 +13859,7 @@
       <c r="V18" s="24"/>
       <c r="W18" s="24"/>
     </row>
-    <row r="19" spans="2:23" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:23" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B19" s="175" t="s">
         <v>620</v>
       </c>
@@ -13885,7 +13885,7 @@
       <c r="V19" s="24"/>
       <c r="W19" s="24"/>
     </row>
-    <row r="20" spans="2:23" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:23" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B20" s="5"/>
       <c r="D20" s="21"/>
       <c r="E20" s="22"/>
@@ -13908,7 +13908,7 @@
       <c r="V20" s="24"/>
       <c r="W20" s="24"/>
     </row>
-    <row r="21" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:23" ht="13" x14ac:dyDescent="0.3">
       <c r="B21" s="52" t="s">
         <v>248</v>
       </c>
@@ -13916,7 +13916,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="22" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B22" s="75" t="s">
         <v>277</v>
       </c>
@@ -13924,7 +13924,7 @@
         <v>400000</v>
       </c>
     </row>
-    <row r="23" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B23" s="51" t="s">
         <v>247</v>
       </c>
@@ -13932,7 +13932,7 @@
         <v>30000</v>
       </c>
     </row>
-    <row r="24" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B24" s="185" t="s">
         <v>626</v>
       </c>
@@ -13946,7 +13946,7 @@
         <v>34050</v>
       </c>
     </row>
-    <row r="25" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B25" s="100" t="s">
         <v>317</v>
       </c>
@@ -13960,7 +13960,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="26" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B26" s="144" t="s">
         <v>446</v>
       </c>
@@ -13972,7 +13972,7 @@
         <v>627</v>
       </c>
     </row>
-    <row r="27" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B27" s="144" t="s">
         <v>447</v>
       </c>
@@ -13983,7 +13983,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="28" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B28" s="51" t="s">
         <v>246</v>
       </c>
@@ -13991,162 +13991,162 @@
         <v>200</v>
       </c>
     </row>
-    <row r="29" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B29" s="100" t="s">
         <v>320</v>
       </c>
     </row>
-    <row r="30" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B30" s="100" t="s">
         <v>322</v>
       </c>
     </row>
-    <row r="31" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B31" s="100" t="s">
         <v>324</v>
       </c>
     </row>
-    <row r="32" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B32" s="100" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B33" s="100" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B34" s="106" t="s">
         <v>350</v>
       </c>
     </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B35" s="51" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B36" s="106" t="s">
         <v>351</v>
       </c>
     </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B37" s="131" t="s">
         <v>404</v>
       </c>
     </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B38" s="106" t="s">
         <v>352</v>
       </c>
     </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B39" s="106" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B40" s="106" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="41" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B41" s="106" t="s">
         <v>354</v>
       </c>
     </row>
-    <row r="42" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B42" s="106" t="s">
         <v>355</v>
       </c>
     </row>
-    <row r="43" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B43" s="106" t="s">
         <v>356</v>
       </c>
     </row>
-    <row r="44" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B44" s="106" t="s">
         <v>357</v>
       </c>
     </row>
-    <row r="45" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B45" s="106" t="s">
         <v>359</v>
       </c>
     </row>
-    <row r="46" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B46" s="106" t="s">
         <v>360</v>
       </c>
     </row>
-    <row r="47" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B47" s="106" t="s">
         <v>361</v>
       </c>
     </row>
-    <row r="48" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B48" s="106" t="s">
         <v>362</v>
       </c>
     </row>
-    <row r="49" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B49" s="106" t="s">
         <v>363</v>
       </c>
     </row>
-    <row r="50" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B50" s="106" t="s">
         <v>364</v>
       </c>
     </row>
-    <row r="51" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B51" s="106" t="s">
         <v>365</v>
       </c>
     </row>
-    <row r="52" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B52" s="106" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="53" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="53" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B53" s="106" t="s">
         <v>367</v>
       </c>
     </row>
-    <row r="54" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="54" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B54" s="106" t="s">
         <v>368</v>
       </c>
     </row>
-    <row r="55" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="55" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B55" s="106" t="s">
         <v>369</v>
       </c>
     </row>
-    <row r="56" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="56" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B56" s="106" t="s">
         <v>370</v>
       </c>
     </row>
-    <row r="57" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="57" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B57" s="106" t="s">
         <v>371</v>
       </c>
     </row>
-    <row r="58" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="58" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B58" s="185" t="s">
         <v>624</v>
       </c>
     </row>
-    <row r="59" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="59" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B59" s="185" t="s">
         <v>628</v>
       </c>
     </row>
-    <row r="60" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="60" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B60" s="185" t="s">
         <v>629</v>
       </c>
@@ -14179,19 +14179,19 @@
       <selection pane="bottomRight" activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5" style="191" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15" style="191" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="191"/>
+    <col min="3" max="16384" width="9.1796875" style="191"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" s="5"/>
       <c r="B2" s="191" t="s">
         <v>0</v>
@@ -14221,7 +14221,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" s="191" t="s">
         <v>253</v>
       </c>
@@ -14270,7 +14270,7 @@
       <c r="V3" s="196"/>
       <c r="W3" s="198"/>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" s="191" t="s">
         <v>253</v>
       </c>
@@ -14314,7 +14314,7 @@
       <c r="V4" s="196"/>
       <c r="W4" s="198"/>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" s="191" t="s">
         <v>253</v>
       </c>
@@ -14361,7 +14361,7 @@
       <c r="V5" s="196"/>
       <c r="W5" s="198"/>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" s="191" t="s">
         <v>253</v>
       </c>
@@ -14411,7 +14411,7 @@
         <v>1982</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" s="191" t="s">
         <v>253</v>
       </c>
@@ -14460,7 +14460,7 @@
       <c r="V7" s="196"/>
       <c r="W7" s="198"/>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B8" s="87" t="s">
         <v>219</v>
       </c>
@@ -14509,7 +14509,7 @@
         <v>1992</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" s="191" t="s">
         <v>253</v>
       </c>
@@ -14526,7 +14526,7 @@
         <v>13640</v>
       </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B10" s="191" t="s">
         <v>222</v>
       </c>
@@ -14558,7 +14558,7 @@
       <c r="V10" s="196"/>
       <c r="W10" s="198"/>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B11" s="191" t="s">
         <v>315</v>
       </c>
@@ -14573,7 +14573,7 @@
       <c r="I11" s="192"/>
       <c r="J11" s="192"/>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B12" s="191" t="s">
         <v>316</v>
       </c>
@@ -14585,7 +14585,7 @@
       <c r="I12" s="192"/>
       <c r="J12" s="192"/>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A13" s="191" t="s">
         <v>253</v>
       </c>
@@ -14596,7 +14596,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A14" s="191" t="s">
         <v>253</v>
       </c>
@@ -14613,7 +14613,7 @@
         <v>13880</v>
       </c>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A15" s="191" t="s">
         <v>253</v>
       </c>
@@ -14624,7 +14624,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A16" s="191" t="s">
         <v>253</v>
       </c>
@@ -14635,7 +14635,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="191" t="s">
         <v>253</v>
       </c>
@@ -14646,7 +14646,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="191" t="s">
         <v>253</v>
       </c>
@@ -14657,7 +14657,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="191" t="s">
         <v>253</v>
       </c>
@@ -14668,7 +14668,7 @@
         <v>556</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="191" t="s">
         <v>253</v>
       </c>
@@ -14679,12 +14679,12 @@
         <v>560</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" ht="13" x14ac:dyDescent="0.3">
       <c r="B22" s="74" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B23" s="191" t="s">
         <v>403</v>
       </c>
@@ -14692,7 +14692,7 @@
         <v>2400</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B24" s="191" t="s">
         <v>382</v>
       </c>
@@ -14700,7 +14700,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B25" s="191" t="s">
         <v>384</v>
       </c>
@@ -14708,7 +14708,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B26" s="191" t="s">
         <v>402</v>
       </c>
@@ -14716,12 +14716,12 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B27" s="191" t="s">
         <v>373</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B28" s="191" t="s">
         <v>383</v>
       </c>

</xml_diff>